<commit_message>
Added getAlignment and setAlignment functions (not quite working yet!)
</commit_message>
<xml_diff>
--- a/data/customXml.xlsx
+++ b/data/customXml.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://tnlcommunityfund-my.sharepoint.com/personal/tim_gebbels_tnlcommunityfund_org_uk/Documents/Documents/Julia Experimenting/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ee85442dac9ca7a7/Documents/Julia/XLSX/XLSX.jl/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="43" documentId="8_{F809508C-CCD6-44EF-B266-70CCB6EF428B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2131C1EA-16BC-4B03-AE4A-1D527D5FABF7}"/>
+  <xr:revisionPtr revIDLastSave="57" documentId="8_{F809508C-CCD6-44EF-B266-70CCB6EF428B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6C875F50-017B-46B0-9F98-DFE4B3507E84}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" tabRatio="604" xr2:uid="{C6551712-42E3-4E24-BA02-CAB261C5432D}"/>
   </bookViews>
@@ -17,6 +17,9 @@
     <sheet name="Document History" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
+    <definedName name="Contiguous">'Mock-up'!$D$23:$D$27</definedName>
+    <definedName name="ID">'Mock-up'!$D$45</definedName>
+    <definedName name="Location">'Mock-up'!$D$18,'Mock-up'!$D$20,'Mock-up'!$J$18,'Mock-up'!$J$20</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="0">'Mock-up'!$A$1:$K$116</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -321,7 +324,7 @@
       <family val="1"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -349,6 +352,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFD9D9D9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.499984740745262"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -666,7 +675,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="74">
+  <cellXfs count="75">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
@@ -818,8 +827,11 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -839,41 +851,41 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -975,6 +987,10 @@
     <mc:Fallback/>
   </mc:AlternateContent>
 </xdr:wsDr>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1279,8 +1295,8 @@
   </sheetPr>
   <dimension ref="A1:K116"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D121" sqref="D121"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="D51" sqref="D51:J53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1414,11 +1430,11 @@
         <v>1</v>
       </c>
       <c r="C9" s="22"/>
-      <c r="D9" s="56"/>
-      <c r="E9" s="56"/>
-      <c r="F9" s="56"/>
-      <c r="G9" s="56"/>
-      <c r="H9" s="56"/>
+      <c r="D9" s="57"/>
+      <c r="E9" s="57"/>
+      <c r="F9" s="57"/>
+      <c r="G9" s="57"/>
+      <c r="H9" s="57"/>
       <c r="I9" s="24"/>
       <c r="J9" s="17"/>
       <c r="K9" s="4"/>
@@ -1442,10 +1458,10 @@
         <v>11</v>
       </c>
       <c r="C11" s="22"/>
-      <c r="D11" s="57"/>
-      <c r="E11" s="58"/>
-      <c r="F11" s="58"/>
-      <c r="G11" s="59"/>
+      <c r="D11" s="58"/>
+      <c r="E11" s="59"/>
+      <c r="F11" s="59"/>
+      <c r="G11" s="60"/>
       <c r="H11" s="17"/>
       <c r="I11" s="17"/>
       <c r="J11" s="13"/>
@@ -1457,10 +1473,10 @@
         <v>12</v>
       </c>
       <c r="C12" s="22"/>
-      <c r="D12" s="57"/>
-      <c r="E12" s="58"/>
-      <c r="F12" s="58"/>
-      <c r="G12" s="59"/>
+      <c r="D12" s="58"/>
+      <c r="E12" s="59"/>
+      <c r="F12" s="59"/>
+      <c r="G12" s="60"/>
       <c r="H12" s="17"/>
       <c r="I12" s="17"/>
       <c r="J12" s="13"/>
@@ -1472,10 +1488,10 @@
         <v>57</v>
       </c>
       <c r="C13" s="22"/>
-      <c r="D13" s="56"/>
-      <c r="E13" s="56"/>
-      <c r="F13" s="56"/>
-      <c r="G13" s="56"/>
+      <c r="D13" s="57"/>
+      <c r="E13" s="57"/>
+      <c r="F13" s="57"/>
+      <c r="G13" s="57"/>
       <c r="H13" s="17"/>
       <c r="I13" s="17"/>
       <c r="J13" s="13"/>
@@ -1487,8 +1503,8 @@
         <v>10</v>
       </c>
       <c r="C14" s="22"/>
-      <c r="D14" s="57"/>
-      <c r="E14" s="59"/>
+      <c r="D14" s="58"/>
+      <c r="E14" s="60"/>
       <c r="F14" s="17"/>
       <c r="G14" s="17"/>
       <c r="H14" s="17"/>
@@ -1515,8 +1531,8 @@
         <v>2</v>
       </c>
       <c r="C16" s="25"/>
-      <c r="D16" s="60"/>
-      <c r="E16" s="61"/>
+      <c r="D16" s="61"/>
+      <c r="E16" s="62"/>
       <c r="F16" s="17"/>
       <c r="G16" s="17"/>
       <c r="H16" s="17"/>
@@ -1543,8 +1559,8 @@
         <v>49</v>
       </c>
       <c r="C18" s="25"/>
-      <c r="D18" s="62"/>
-      <c r="E18" s="63"/>
+      <c r="D18" s="63"/>
+      <c r="E18" s="64"/>
       <c r="F18" s="17"/>
       <c r="G18" s="17"/>
       <c r="H18" s="21" t="s">
@@ -1573,8 +1589,8 @@
         <v>51</v>
       </c>
       <c r="C20" s="25"/>
-      <c r="D20" s="62"/>
-      <c r="E20" s="63"/>
+      <c r="D20" s="63"/>
+      <c r="E20" s="64"/>
       <c r="F20" s="17"/>
       <c r="G20" s="17"/>
       <c r="H20" s="21" t="s">
@@ -1745,9 +1761,9 @@
         <v>26</v>
       </c>
       <c r="C32" s="22"/>
-      <c r="D32" s="56"/>
-      <c r="E32" s="56"/>
-      <c r="F32" s="56"/>
+      <c r="D32" s="57"/>
+      <c r="E32" s="57"/>
+      <c r="F32" s="57"/>
       <c r="G32" s="17"/>
       <c r="H32" s="17"/>
       <c r="I32" s="17"/>
@@ -1773,13 +1789,13 @@
         <v>29</v>
       </c>
       <c r="C34" s="28"/>
-      <c r="D34" s="56"/>
-      <c r="E34" s="56"/>
-      <c r="F34" s="56"/>
-      <c r="G34" s="56"/>
-      <c r="H34" s="56"/>
-      <c r="I34" s="56"/>
-      <c r="J34" s="56"/>
+      <c r="D34" s="57"/>
+      <c r="E34" s="57"/>
+      <c r="F34" s="57"/>
+      <c r="G34" s="57"/>
+      <c r="H34" s="57"/>
+      <c r="I34" s="57"/>
+      <c r="J34" s="57"/>
       <c r="K34" s="4"/>
     </row>
     <row r="35" spans="1:11" ht="6" customHeight="1" x14ac:dyDescent="0.25">
@@ -1831,13 +1847,13 @@
         <v>34</v>
       </c>
       <c r="C38" s="28"/>
-      <c r="D38" s="56"/>
-      <c r="E38" s="56"/>
-      <c r="F38" s="56"/>
-      <c r="G38" s="56"/>
-      <c r="H38" s="56"/>
-      <c r="I38" s="56"/>
-      <c r="J38" s="56"/>
+      <c r="D38" s="57"/>
+      <c r="E38" s="57"/>
+      <c r="F38" s="57"/>
+      <c r="G38" s="57"/>
+      <c r="H38" s="57"/>
+      <c r="I38" s="57"/>
+      <c r="J38" s="57"/>
       <c r="K38" s="4"/>
     </row>
     <row r="39" spans="1:11" ht="6" customHeight="1" x14ac:dyDescent="0.25">
@@ -1930,7 +1946,7 @@
         <v>35</v>
       </c>
       <c r="C45" s="22"/>
-      <c r="D45" s="25"/>
+      <c r="D45" s="56"/>
       <c r="E45" s="17"/>
       <c r="F45" s="13"/>
       <c r="G45" s="13"/>
@@ -1960,11 +1976,11 @@
         <v>37</v>
       </c>
       <c r="C47" s="25"/>
-      <c r="D47" s="56"/>
-      <c r="E47" s="56"/>
-      <c r="F47" s="56"/>
-      <c r="G47" s="56"/>
-      <c r="H47" s="56"/>
+      <c r="D47" s="57"/>
+      <c r="E47" s="57"/>
+      <c r="F47" s="57"/>
+      <c r="G47" s="57"/>
+      <c r="H47" s="57"/>
       <c r="I47" s="17"/>
       <c r="J47" s="32"/>
       <c r="K47" s="4"/>
@@ -1988,11 +2004,11 @@
         <v>36</v>
       </c>
       <c r="C49" s="22"/>
-      <c r="D49" s="57"/>
-      <c r="E49" s="58"/>
-      <c r="F49" s="58"/>
-      <c r="G49" s="58"/>
-      <c r="H49" s="59"/>
+      <c r="D49" s="58"/>
+      <c r="E49" s="59"/>
+      <c r="F49" s="59"/>
+      <c r="G49" s="59"/>
+      <c r="H49" s="60"/>
       <c r="I49" s="24"/>
       <c r="J49" s="32"/>
       <c r="K49" s="4"/>
@@ -2016,39 +2032,39 @@
         <v>7</v>
       </c>
       <c r="C51" s="22"/>
-      <c r="D51" s="65"/>
-      <c r="E51" s="66"/>
-      <c r="F51" s="66"/>
-      <c r="G51" s="66"/>
-      <c r="H51" s="66"/>
-      <c r="I51" s="66"/>
-      <c r="J51" s="67"/>
+      <c r="D51" s="66"/>
+      <c r="E51" s="67"/>
+      <c r="F51" s="67"/>
+      <c r="G51" s="67"/>
+      <c r="H51" s="67"/>
+      <c r="I51" s="67"/>
+      <c r="J51" s="68"/>
       <c r="K51" s="4"/>
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A52" s="3"/>
       <c r="B52" s="17"/>
       <c r="C52" s="17"/>
-      <c r="D52" s="71"/>
-      <c r="E52" s="72"/>
-      <c r="F52" s="72"/>
-      <c r="G52" s="72"/>
-      <c r="H52" s="72"/>
-      <c r="I52" s="72"/>
-      <c r="J52" s="73"/>
+      <c r="D52" s="72"/>
+      <c r="E52" s="73"/>
+      <c r="F52" s="73"/>
+      <c r="G52" s="73"/>
+      <c r="H52" s="73"/>
+      <c r="I52" s="73"/>
+      <c r="J52" s="74"/>
       <c r="K52" s="4"/>
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A53" s="3"/>
       <c r="B53" s="17"/>
       <c r="C53" s="17"/>
-      <c r="D53" s="68"/>
-      <c r="E53" s="69"/>
-      <c r="F53" s="69"/>
-      <c r="G53" s="69"/>
-      <c r="H53" s="69"/>
-      <c r="I53" s="69"/>
-      <c r="J53" s="70"/>
+      <c r="D53" s="69"/>
+      <c r="E53" s="70"/>
+      <c r="F53" s="70"/>
+      <c r="G53" s="70"/>
+      <c r="H53" s="70"/>
+      <c r="I53" s="70"/>
+      <c r="J53" s="71"/>
       <c r="K53" s="4"/>
     </row>
     <row r="54" spans="1:11" x14ac:dyDescent="0.25">
@@ -2070,78 +2086,78 @@
         <v>8</v>
       </c>
       <c r="C55" s="22"/>
-      <c r="D55" s="65"/>
-      <c r="E55" s="66"/>
-      <c r="F55" s="66"/>
-      <c r="G55" s="66"/>
-      <c r="H55" s="66"/>
-      <c r="I55" s="66"/>
-      <c r="J55" s="67"/>
+      <c r="D55" s="66"/>
+      <c r="E55" s="67"/>
+      <c r="F55" s="67"/>
+      <c r="G55" s="67"/>
+      <c r="H55" s="67"/>
+      <c r="I55" s="67"/>
+      <c r="J55" s="68"/>
       <c r="K55" s="4"/>
     </row>
     <row r="56" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A56" s="3"/>
       <c r="B56" s="33"/>
       <c r="C56" s="17"/>
-      <c r="D56" s="71"/>
-      <c r="E56" s="72"/>
-      <c r="F56" s="72"/>
-      <c r="G56" s="72"/>
-      <c r="H56" s="72"/>
-      <c r="I56" s="72"/>
-      <c r="J56" s="73"/>
+      <c r="D56" s="72"/>
+      <c r="E56" s="73"/>
+      <c r="F56" s="73"/>
+      <c r="G56" s="73"/>
+      <c r="H56" s="73"/>
+      <c r="I56" s="73"/>
+      <c r="J56" s="74"/>
       <c r="K56" s="4"/>
     </row>
     <row r="57" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A57" s="3"/>
       <c r="B57" s="33"/>
       <c r="C57" s="17"/>
-      <c r="D57" s="71"/>
-      <c r="E57" s="72"/>
-      <c r="F57" s="72"/>
-      <c r="G57" s="72"/>
-      <c r="H57" s="72"/>
-      <c r="I57" s="72"/>
-      <c r="J57" s="73"/>
+      <c r="D57" s="72"/>
+      <c r="E57" s="73"/>
+      <c r="F57" s="73"/>
+      <c r="G57" s="73"/>
+      <c r="H57" s="73"/>
+      <c r="I57" s="73"/>
+      <c r="J57" s="74"/>
       <c r="K57" s="4"/>
     </row>
     <row r="58" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A58" s="3"/>
       <c r="B58" s="33"/>
       <c r="C58" s="17"/>
-      <c r="D58" s="71"/>
-      <c r="E58" s="72"/>
-      <c r="F58" s="72"/>
-      <c r="G58" s="72"/>
-      <c r="H58" s="72"/>
-      <c r="I58" s="72"/>
-      <c r="J58" s="73"/>
+      <c r="D58" s="72"/>
+      <c r="E58" s="73"/>
+      <c r="F58" s="73"/>
+      <c r="G58" s="73"/>
+      <c r="H58" s="73"/>
+      <c r="I58" s="73"/>
+      <c r="J58" s="74"/>
       <c r="K58" s="4"/>
     </row>
     <row r="59" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A59" s="3"/>
       <c r="B59" s="17"/>
       <c r="C59" s="17"/>
-      <c r="D59" s="71"/>
-      <c r="E59" s="72"/>
-      <c r="F59" s="72"/>
-      <c r="G59" s="72"/>
-      <c r="H59" s="72"/>
-      <c r="I59" s="72"/>
-      <c r="J59" s="73"/>
+      <c r="D59" s="72"/>
+      <c r="E59" s="73"/>
+      <c r="F59" s="73"/>
+      <c r="G59" s="73"/>
+      <c r="H59" s="73"/>
+      <c r="I59" s="73"/>
+      <c r="J59" s="74"/>
       <c r="K59" s="4"/>
     </row>
     <row r="60" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A60" s="3"/>
       <c r="B60" s="17"/>
       <c r="C60" s="17"/>
-      <c r="D60" s="68"/>
-      <c r="E60" s="69"/>
-      <c r="F60" s="69"/>
-      <c r="G60" s="69"/>
-      <c r="H60" s="69"/>
-      <c r="I60" s="69"/>
-      <c r="J60" s="70"/>
+      <c r="D60" s="69"/>
+      <c r="E60" s="70"/>
+      <c r="F60" s="70"/>
+      <c r="G60" s="70"/>
+      <c r="H60" s="70"/>
+      <c r="I60" s="70"/>
+      <c r="J60" s="71"/>
       <c r="K60" s="4"/>
     </row>
     <row r="61" spans="1:11" x14ac:dyDescent="0.25">
@@ -2163,26 +2179,26 @@
         <v>16</v>
       </c>
       <c r="C62" s="22"/>
-      <c r="D62" s="65"/>
-      <c r="E62" s="66"/>
-      <c r="F62" s="66"/>
-      <c r="G62" s="66"/>
-      <c r="H62" s="66"/>
-      <c r="I62" s="66"/>
-      <c r="J62" s="67"/>
+      <c r="D62" s="66"/>
+      <c r="E62" s="67"/>
+      <c r="F62" s="67"/>
+      <c r="G62" s="67"/>
+      <c r="H62" s="67"/>
+      <c r="I62" s="67"/>
+      <c r="J62" s="68"/>
       <c r="K62" s="4"/>
     </row>
     <row r="63" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A63" s="3"/>
       <c r="B63" s="34"/>
       <c r="C63" s="34"/>
-      <c r="D63" s="68"/>
-      <c r="E63" s="69"/>
-      <c r="F63" s="69"/>
-      <c r="G63" s="69"/>
-      <c r="H63" s="69"/>
-      <c r="I63" s="69"/>
-      <c r="J63" s="70"/>
+      <c r="D63" s="69"/>
+      <c r="E63" s="70"/>
+      <c r="F63" s="70"/>
+      <c r="G63" s="70"/>
+      <c r="H63" s="70"/>
+      <c r="I63" s="70"/>
+      <c r="J63" s="71"/>
       <c r="K63" s="4"/>
     </row>
     <row r="64" spans="1:11" ht="6" customHeight="1" x14ac:dyDescent="0.25">
@@ -2234,26 +2250,26 @@
         <v>19</v>
       </c>
       <c r="C67" s="22"/>
-      <c r="D67" s="65"/>
-      <c r="E67" s="66"/>
-      <c r="F67" s="66"/>
-      <c r="G67" s="66"/>
-      <c r="H67" s="66"/>
-      <c r="I67" s="66"/>
-      <c r="J67" s="67"/>
+      <c r="D67" s="66"/>
+      <c r="E67" s="67"/>
+      <c r="F67" s="67"/>
+      <c r="G67" s="67"/>
+      <c r="H67" s="67"/>
+      <c r="I67" s="67"/>
+      <c r="J67" s="68"/>
       <c r="K67" s="4"/>
     </row>
     <row r="68" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A68" s="3"/>
       <c r="B68" s="34"/>
       <c r="C68" s="34"/>
-      <c r="D68" s="68"/>
-      <c r="E68" s="69"/>
-      <c r="F68" s="69"/>
-      <c r="G68" s="69"/>
-      <c r="H68" s="69"/>
-      <c r="I68" s="69"/>
-      <c r="J68" s="70"/>
+      <c r="D68" s="69"/>
+      <c r="E68" s="70"/>
+      <c r="F68" s="70"/>
+      <c r="G68" s="70"/>
+      <c r="H68" s="70"/>
+      <c r="I68" s="70"/>
+      <c r="J68" s="71"/>
       <c r="K68" s="4"/>
     </row>
     <row r="69" spans="1:11" ht="6" customHeight="1" x14ac:dyDescent="0.25">
@@ -2305,13 +2321,13 @@
         <v>9</v>
       </c>
       <c r="C72" s="22"/>
-      <c r="D72" s="57"/>
-      <c r="E72" s="58"/>
-      <c r="F72" s="58"/>
-      <c r="G72" s="58"/>
-      <c r="H72" s="58"/>
-      <c r="I72" s="58"/>
-      <c r="J72" s="59"/>
+      <c r="D72" s="58"/>
+      <c r="E72" s="59"/>
+      <c r="F72" s="59"/>
+      <c r="G72" s="59"/>
+      <c r="H72" s="59"/>
+      <c r="I72" s="59"/>
+      <c r="J72" s="60"/>
       <c r="K72" s="4"/>
     </row>
     <row r="73" spans="1:11" x14ac:dyDescent="0.25">
@@ -2333,13 +2349,13 @@
         <v>13</v>
       </c>
       <c r="C74" s="22"/>
-      <c r="D74" s="56"/>
-      <c r="E74" s="56"/>
-      <c r="F74" s="56"/>
-      <c r="G74" s="56"/>
-      <c r="H74" s="56"/>
-      <c r="I74" s="56"/>
-      <c r="J74" s="56"/>
+      <c r="D74" s="57"/>
+      <c r="E74" s="57"/>
+      <c r="F74" s="57"/>
+      <c r="G74" s="57"/>
+      <c r="H74" s="57"/>
+      <c r="I74" s="57"/>
+      <c r="J74" s="57"/>
       <c r="K74" s="4"/>
     </row>
     <row r="75" spans="1:11" x14ac:dyDescent="0.25">
@@ -2453,13 +2469,13 @@
         <v>38</v>
       </c>
       <c r="C82" s="37"/>
-      <c r="D82" s="56"/>
-      <c r="E82" s="56"/>
-      <c r="F82" s="56"/>
-      <c r="G82" s="56"/>
-      <c r="H82" s="56"/>
-      <c r="I82" s="56"/>
-      <c r="J82" s="56"/>
+      <c r="D82" s="57"/>
+      <c r="E82" s="57"/>
+      <c r="F82" s="57"/>
+      <c r="G82" s="57"/>
+      <c r="H82" s="57"/>
+      <c r="I82" s="57"/>
+      <c r="J82" s="57"/>
       <c r="K82" s="4"/>
     </row>
     <row r="83" spans="1:11" ht="6" customHeight="1" x14ac:dyDescent="0.25">
@@ -2483,11 +2499,11 @@
         <v>22</v>
       </c>
       <c r="E84" s="22"/>
-      <c r="F84" s="64"/>
-      <c r="G84" s="64"/>
-      <c r="H84" s="64"/>
-      <c r="I84" s="64"/>
-      <c r="J84" s="64"/>
+      <c r="F84" s="65"/>
+      <c r="G84" s="65"/>
+      <c r="H84" s="65"/>
+      <c r="I84" s="65"/>
+      <c r="J84" s="65"/>
       <c r="K84" s="4"/>
     </row>
     <row r="85" spans="1:11" ht="6" customHeight="1" x14ac:dyDescent="0.25">
@@ -2511,11 +2527,11 @@
         <v>20</v>
       </c>
       <c r="E86" s="22"/>
-      <c r="F86" s="64"/>
-      <c r="G86" s="64"/>
-      <c r="H86" s="64"/>
-      <c r="I86" s="64"/>
-      <c r="J86" s="64"/>
+      <c r="F86" s="65"/>
+      <c r="G86" s="65"/>
+      <c r="H86" s="65"/>
+      <c r="I86" s="65"/>
+      <c r="J86" s="65"/>
       <c r="K86" s="4"/>
     </row>
     <row r="87" spans="1:11" ht="6" customHeight="1" x14ac:dyDescent="0.25">
@@ -2595,13 +2611,13 @@
         <v>39</v>
       </c>
       <c r="C92" s="37"/>
-      <c r="D92" s="56"/>
-      <c r="E92" s="56"/>
-      <c r="F92" s="56"/>
-      <c r="G92" s="56"/>
-      <c r="H92" s="56"/>
-      <c r="I92" s="56"/>
-      <c r="J92" s="56"/>
+      <c r="D92" s="57"/>
+      <c r="E92" s="57"/>
+      <c r="F92" s="57"/>
+      <c r="G92" s="57"/>
+      <c r="H92" s="57"/>
+      <c r="I92" s="57"/>
+      <c r="J92" s="57"/>
       <c r="K92" s="4"/>
     </row>
     <row r="93" spans="1:11" ht="6" customHeight="1" x14ac:dyDescent="0.25">
@@ -2625,11 +2641,11 @@
         <v>22</v>
       </c>
       <c r="E94" s="22"/>
-      <c r="F94" s="64"/>
-      <c r="G94" s="64"/>
-      <c r="H94" s="64"/>
-      <c r="I94" s="64"/>
-      <c r="J94" s="64"/>
+      <c r="F94" s="65"/>
+      <c r="G94" s="65"/>
+      <c r="H94" s="65"/>
+      <c r="I94" s="65"/>
+      <c r="J94" s="65"/>
       <c r="K94" s="4"/>
     </row>
     <row r="95" spans="1:11" ht="6" customHeight="1" x14ac:dyDescent="0.25">
@@ -2653,11 +2669,11 @@
         <v>20</v>
       </c>
       <c r="E96" s="22"/>
-      <c r="F96" s="64"/>
-      <c r="G96" s="64"/>
-      <c r="H96" s="64"/>
-      <c r="I96" s="64"/>
-      <c r="J96" s="64"/>
+      <c r="F96" s="65"/>
+      <c r="G96" s="65"/>
+      <c r="H96" s="65"/>
+      <c r="I96" s="65"/>
+      <c r="J96" s="65"/>
       <c r="K96" s="4"/>
     </row>
     <row r="97" spans="1:11" ht="6" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Support merging of cells (#241 & #184)
</commit_message>
<xml_diff>
--- a/data/customXml.xlsx
+++ b/data/customXml.xlsx
@@ -18,10 +18,10 @@
   </sheets>
   <definedNames>
     <definedName name="Contiguous">'Mock-up'!$D$23:$D$27</definedName>
+    <definedName name="Location">'Mock-up'!$D$18,'Mock-up'!$D$20,'Mock-up'!$J$18,'Mock-up'!$J$20</definedName>
+    <definedName name="Short_Description">'Mock-up'!$D$51</definedName>
     <definedName name="ID">'Mock-up'!$D$45</definedName>
-    <definedName name="Location">'Mock-up'!$D$18,'Mock-up'!$D$20,'Mock-up'!$J$18,'Mock-up'!$J$20</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="0">'Mock-up'!$A$1:$K$116</definedName>
-    <definedName name="Short_Description" comment="This is some text">'Mock-up'!$D$51</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="69">
   <si>
     <t>Recipient ID</t>
   </si>
@@ -121,7 +121,7 @@
     <t>Comment</t>
   </si>
   <si>
-    <t xml:space="preserve">Date </t>
+    <t xml:space="preserve">Date</t>
   </si>
   <si>
     <t>Distributor</t>
@@ -238,7 +238,7 @@
     <t>Competition Details</t>
   </si>
   <si>
-    <t xml:space="preserve">First draft to stimulate feedback </t>
+    <t xml:space="preserve">First draft to stimulate feedback</t>
   </si>
   <si>
     <t>Revised to show suggested mandatory / optional fields. Changed title.</t>
@@ -986,7 +986,7 @@
                   <a:latin typeface="Segoe UI"/>
                   <a:cs typeface="Segoe UI"/>
                 </a:rPr>
-                <a:t> </a:t>
+                <a:t/>
               </a:r>
             </a:p>
           </xdr:txBody>
@@ -1333,9 +1333,9 @@
       <c r="J1" s="15"/>
       <c r="K1" s="2"/>
     </row>
-    <row r="2" spans="1:11" ht="23.25" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3"/>
-      <c r="B2" s="16" t="s">
+      <c r="B2" t="s" s="16">
         <v>62</v>
       </c>
       <c r="C2" s="17"/>
@@ -1348,7 +1348,7 @@
       <c r="J2" s="17"/>
       <c r="K2" s="4"/>
     </row>
-    <row r="3" spans="1:11" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" ht="6.0" customHeight="1" x14ac:dyDescent="0.3" thickBot="1">
       <c r="A3" s="5"/>
       <c r="B3" s="18"/>
       <c r="C3" s="19"/>
@@ -1361,7 +1361,7 @@
       <c r="J3" s="19"/>
       <c r="K3" s="6"/>
     </row>
-    <row r="4" spans="1:11" ht="6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" ht="6.0" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3"/>
       <c r="B4" s="16"/>
       <c r="C4" s="17"/>
@@ -1374,9 +1374,9 @@
       <c r="J4" s="17"/>
       <c r="K4" s="4"/>
     </row>
-    <row r="5" spans="1:11" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" ht="18.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3"/>
-      <c r="B5" s="20" t="s">
+      <c r="B5" t="s" s="20">
         <v>61</v>
       </c>
       <c r="C5" s="17"/>
@@ -1404,7 +1404,7 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="3"/>
-      <c r="B7" s="21" t="s">
+      <c r="B7" t="s" s="21">
         <v>0</v>
       </c>
       <c r="C7" s="22"/>
@@ -1432,7 +1432,7 @@
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="3"/>
-      <c r="B9" s="21" t="s">
+      <c r="B9" t="s" s="21">
         <v>1</v>
       </c>
       <c r="C9" s="22"/>
@@ -1460,7 +1460,7 @@
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="3"/>
-      <c r="B11" s="21" t="s">
+      <c r="B11" t="s" s="21">
         <v>11</v>
       </c>
       <c r="C11" s="22"/>
@@ -1475,7 +1475,7 @@
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="3"/>
-      <c r="B12" s="21" t="s">
+      <c r="B12" t="s" s="21">
         <v>12</v>
       </c>
       <c r="C12" s="22"/>
@@ -1490,7 +1490,7 @@
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="3"/>
-      <c r="B13" s="21" t="s">
+      <c r="B13" t="s" s="21">
         <v>57</v>
       </c>
       <c r="C13" s="22"/>
@@ -1505,7 +1505,7 @@
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="3"/>
-      <c r="B14" s="21" t="s">
+      <c r="B14" t="s" s="21">
         <v>10</v>
       </c>
       <c r="C14" s="22"/>
@@ -1533,7 +1533,7 @@
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="3"/>
-      <c r="B16" s="21" t="s">
+      <c r="B16" t="s" s="21">
         <v>2</v>
       </c>
       <c r="C16" s="25"/>
@@ -1561,24 +1561,24 @@
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="3"/>
-      <c r="B18" s="21" t="s">
+      <c r="B18" t="s" s="21">
         <v>49</v>
       </c>
       <c r="C18" s="25"/>
-      <c r="D18" s="63" t="s">
+      <c r="D18" t="s" s="63">
         <v>68</v>
       </c>
       <c r="E18" s="64"/>
       <c r="F18" s="17"/>
       <c r="G18" s="17"/>
-      <c r="H18" s="21" t="s">
+      <c r="H18" t="s" s="21">
         <v>50</v>
       </c>
       <c r="I18" s="25"/>
       <c r="J18" s="55"/>
       <c r="K18" s="4"/>
     </row>
-    <row r="19" spans="1:11" ht="6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" ht="6.0" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="3"/>
       <c r="B19" s="17"/>
       <c r="C19" s="17"/>
@@ -1593,7 +1593,7 @@
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="3"/>
-      <c r="B20" s="21" t="s">
+      <c r="B20" t="s" s="21">
         <v>51</v>
       </c>
       <c r="C20" s="25"/>
@@ -1601,7 +1601,7 @@
       <c r="E20" s="64"/>
       <c r="F20" s="17"/>
       <c r="G20" s="17"/>
-      <c r="H20" s="21" t="s">
+      <c r="H20" t="s" s="21">
         <v>52</v>
       </c>
       <c r="I20" s="25"/>
@@ -1623,23 +1623,23 @@
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="3"/>
-      <c r="B22" s="21" t="s">
+      <c r="B22" t="s" s="21">
         <v>3</v>
       </c>
       <c r="C22" s="26"/>
-      <c r="D22" s="21" t="s">
+      <c r="D22" t="s" s="21">
         <v>5</v>
       </c>
       <c r="E22" s="26"/>
-      <c r="F22" s="21" t="s">
+      <c r="F22" t="s" s="21">
         <v>6</v>
       </c>
       <c r="G22" s="26"/>
-      <c r="H22" s="21" t="s">
+      <c r="H22" t="s" s="21">
         <v>4</v>
       </c>
       <c r="I22" s="22"/>
-      <c r="J22" s="21" t="s">
+      <c r="J22" t="s" s="21">
         <v>26</v>
       </c>
       <c r="K22" s="4"/>
@@ -1709,7 +1709,7 @@
       <c r="J27" s="21"/>
       <c r="K27" s="4"/>
     </row>
-    <row r="28" spans="1:11" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:11" ht="6.0" customHeight="1" x14ac:dyDescent="0.3" thickBot="1">
       <c r="A28" s="5"/>
       <c r="B28" s="19"/>
       <c r="C28" s="19"/>
@@ -1722,7 +1722,7 @@
       <c r="J28" s="27"/>
       <c r="K28" s="6"/>
     </row>
-    <row r="29" spans="1:11" ht="6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" ht="6.0" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="3"/>
       <c r="B29" s="17"/>
       <c r="C29" s="17"/>
@@ -1735,9 +1735,9 @@
       <c r="J29" s="24"/>
       <c r="K29" s="4"/>
     </row>
-    <row r="30" spans="1:11" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="3"/>
-      <c r="B30" s="20" t="s">
+      <c r="B30" t="s" s="20">
         <v>33</v>
       </c>
       <c r="C30" s="17"/>
@@ -1765,7 +1765,7 @@
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="3"/>
-      <c r="B32" s="21" t="s">
+      <c r="B32" t="s" s="21">
         <v>26</v>
       </c>
       <c r="C32" s="22"/>
@@ -1793,7 +1793,7 @@
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" s="3"/>
-      <c r="B34" s="21" t="s">
+      <c r="B34" t="s" s="21">
         <v>29</v>
       </c>
       <c r="C34" s="28"/>
@@ -1806,7 +1806,7 @@
       <c r="J34" s="57"/>
       <c r="K34" s="4"/>
     </row>
-    <row r="35" spans="1:11" ht="6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:11" ht="6.0" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="3"/>
       <c r="B35" s="17"/>
       <c r="C35" s="17"/>
@@ -1823,13 +1823,13 @@
       <c r="A36" s="3"/>
       <c r="B36" s="17"/>
       <c r="C36" s="17"/>
-      <c r="D36" s="21" t="s">
+      <c r="D36" t="s" s="21">
         <v>31</v>
       </c>
       <c r="E36" s="22"/>
       <c r="F36" s="21"/>
       <c r="G36" s="30"/>
-      <c r="H36" s="21" t="s">
+      <c r="H36" t="s" s="21">
         <v>30</v>
       </c>
       <c r="I36" s="22"/>
@@ -1851,7 +1851,7 @@
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" s="3"/>
-      <c r="B38" s="21" t="s">
+      <c r="B38" t="s" s="21">
         <v>34</v>
       </c>
       <c r="C38" s="28"/>
@@ -1864,7 +1864,7 @@
       <c r="J38" s="57"/>
       <c r="K38" s="4"/>
     </row>
-    <row r="39" spans="1:11" ht="6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:11" ht="6.0" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="3"/>
       <c r="B39" s="17"/>
       <c r="C39" s="17"/>
@@ -1881,20 +1881,20 @@
       <c r="A40" s="3"/>
       <c r="B40" s="17"/>
       <c r="C40" s="17"/>
-      <c r="D40" s="21" t="s">
+      <c r="D40" t="s" s="21">
         <v>31</v>
       </c>
       <c r="E40" s="25"/>
       <c r="F40" s="21"/>
       <c r="G40" s="30"/>
-      <c r="H40" s="21" t="s">
+      <c r="H40" t="s" s="21">
         <v>28</v>
       </c>
       <c r="I40" s="25"/>
       <c r="J40" s="21"/>
       <c r="K40" s="4"/>
     </row>
-    <row r="41" spans="1:11" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:11" ht="6.0" customHeight="1" x14ac:dyDescent="0.3" thickBot="1">
       <c r="A41" s="5"/>
       <c r="B41" s="19"/>
       <c r="C41" s="19"/>
@@ -1907,7 +1907,7 @@
       <c r="J41" s="27"/>
       <c r="K41" s="6"/>
     </row>
-    <row r="42" spans="1:11" ht="6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:11" ht="6.0" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="3"/>
       <c r="B42" s="17"/>
       <c r="C42" s="17"/>
@@ -1920,9 +1920,9 @@
       <c r="J42" s="24"/>
       <c r="K42" s="4"/>
     </row>
-    <row r="43" spans="1:11" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="3"/>
-      <c r="B43" s="20" t="s">
+      <c r="B43" t="s" s="20">
         <v>60</v>
       </c>
       <c r="C43" s="17"/>
@@ -1950,7 +1950,7 @@
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45" s="3"/>
-      <c r="B45" s="21" t="s">
+      <c r="B45" t="s" s="21">
         <v>35</v>
       </c>
       <c r="C45" s="22"/>
@@ -1958,7 +1958,7 @@
       <c r="E45" s="17"/>
       <c r="F45" s="13"/>
       <c r="G45" s="13"/>
-      <c r="H45" s="21" t="s">
+      <c r="H45" t="s" s="21">
         <v>48</v>
       </c>
       <c r="I45" s="22"/>
@@ -1980,7 +1980,7 @@
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A47" s="3"/>
-      <c r="B47" s="21" t="s">
+      <c r="B47" t="s" s="21">
         <v>37</v>
       </c>
       <c r="C47" s="25"/>
@@ -2008,7 +2008,7 @@
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A49" s="3"/>
-      <c r="B49" s="21" t="s">
+      <c r="B49" t="s" s="21">
         <v>36</v>
       </c>
       <c r="C49" s="22"/>
@@ -2036,11 +2036,11 @@
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A51" s="3"/>
-      <c r="B51" s="21" t="s">
+      <c r="B51" t="s" s="21">
         <v>7</v>
       </c>
       <c r="C51" s="22"/>
-      <c r="D51" s="67" t="s">
+      <c r="D51" t="s" s="67">
         <v>67</v>
       </c>
       <c r="E51" s="68"/>
@@ -2092,7 +2092,7 @@
     </row>
     <row r="55" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A55" s="3"/>
-      <c r="B55" s="21" t="s">
+      <c r="B55" t="s" s="21">
         <v>8</v>
       </c>
       <c r="C55" s="22"/>
@@ -2185,7 +2185,7 @@
     </row>
     <row r="62" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A62" s="3"/>
-      <c r="B62" s="21" t="s">
+      <c r="B62" t="s" s="21">
         <v>16</v>
       </c>
       <c r="C62" s="22"/>
@@ -2211,7 +2211,7 @@
       <c r="J63" s="72"/>
       <c r="K63" s="4"/>
     </row>
-    <row r="64" spans="1:11" ht="6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:11" ht="6.0" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="3"/>
       <c r="B64" s="17"/>
       <c r="C64" s="17"/>
@@ -2228,13 +2228,13 @@
       <c r="A65" s="3"/>
       <c r="B65" s="17"/>
       <c r="C65" s="17"/>
-      <c r="D65" s="21" t="s">
+      <c r="D65" t="s" s="21">
         <v>17</v>
       </c>
       <c r="E65" s="22"/>
       <c r="F65" s="21"/>
       <c r="G65" s="35"/>
-      <c r="H65" s="21" t="s">
+      <c r="H65" t="s" s="21">
         <v>18</v>
       </c>
       <c r="I65" s="22"/>
@@ -2256,7 +2256,7 @@
     </row>
     <row r="67" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A67" s="3"/>
-      <c r="B67" s="21" t="s">
+      <c r="B67" t="s" s="21">
         <v>19</v>
       </c>
       <c r="C67" s="22"/>
@@ -2282,7 +2282,7 @@
       <c r="J68" s="72"/>
       <c r="K68" s="4"/>
     </row>
-    <row r="69" spans="1:11" ht="6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:11" ht="6.0" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="3"/>
       <c r="B69" s="17"/>
       <c r="C69" s="17"/>
@@ -2299,13 +2299,13 @@
       <c r="A70" s="3"/>
       <c r="B70" s="17"/>
       <c r="C70" s="17"/>
-      <c r="D70" s="21" t="s">
+      <c r="D70" t="s" s="21">
         <v>17</v>
       </c>
       <c r="E70" s="25"/>
       <c r="F70" s="21"/>
       <c r="G70" s="36"/>
-      <c r="H70" s="21" t="s">
+      <c r="H70" t="s" s="21">
         <v>18</v>
       </c>
       <c r="I70" s="22"/>
@@ -2327,7 +2327,7 @@
     </row>
     <row r="72" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A72" s="3"/>
-      <c r="B72" s="21" t="s">
+      <c r="B72" t="s" s="21">
         <v>9</v>
       </c>
       <c r="C72" s="22"/>
@@ -2357,7 +2357,7 @@
     </row>
     <row r="74" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A74" s="3"/>
-      <c r="B74" s="21" t="s">
+      <c r="B74" t="s" s="21">
         <v>13</v>
       </c>
       <c r="C74" s="22"/>
@@ -2385,24 +2385,24 @@
     </row>
     <row r="76" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A76" s="3"/>
-      <c r="B76" s="21" t="s">
+      <c r="B76" t="s" s="21">
         <v>46</v>
       </c>
       <c r="C76" s="22"/>
-      <c r="D76" s="21" t="s">
+      <c r="D76" t="s" s="21">
         <v>41</v>
       </c>
       <c r="E76" s="25"/>
       <c r="F76" s="21"/>
       <c r="G76" s="52"/>
-      <c r="H76" s="21" t="s">
+      <c r="H76" t="s" s="21">
         <v>47</v>
       </c>
       <c r="I76" s="22"/>
       <c r="J76" s="21"/>
       <c r="K76" s="4"/>
     </row>
-    <row r="77" spans="1:11" ht="6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:11" ht="6.0" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" s="3"/>
       <c r="B77" s="17"/>
       <c r="C77" s="17"/>
@@ -2419,20 +2419,20 @@
       <c r="A78" s="3"/>
       <c r="B78" s="17"/>
       <c r="C78" s="17"/>
-      <c r="D78" s="21" t="s">
+      <c r="D78" t="s" s="21">
         <v>42</v>
       </c>
       <c r="E78" s="25"/>
       <c r="F78" s="21"/>
       <c r="G78" s="51"/>
-      <c r="H78" s="21" t="s">
+      <c r="H78" t="s" s="21">
         <v>44</v>
       </c>
       <c r="I78" s="22"/>
       <c r="J78" s="21"/>
       <c r="K78" s="4"/>
     </row>
-    <row r="79" spans="1:11" ht="6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:11" ht="6.0" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" s="3"/>
       <c r="B79" s="17"/>
       <c r="C79" s="17"/>
@@ -2449,13 +2449,13 @@
       <c r="A80" s="3"/>
       <c r="B80" s="17"/>
       <c r="C80" s="17"/>
-      <c r="D80" s="21" t="s">
+      <c r="D80" t="s" s="21">
         <v>43</v>
       </c>
       <c r="E80" s="25"/>
       <c r="F80" s="21"/>
       <c r="G80" s="36"/>
-      <c r="H80" s="21" t="s">
+      <c r="H80" t="s" s="21">
         <v>45</v>
       </c>
       <c r="I80" s="22"/>
@@ -2477,7 +2477,7 @@
     </row>
     <row r="82" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A82" s="3"/>
-      <c r="B82" s="21" t="s">
+      <c r="B82" t="s" s="21">
         <v>38</v>
       </c>
       <c r="C82" s="37"/>
@@ -2490,7 +2490,7 @@
       <c r="J82" s="57"/>
       <c r="K82" s="4"/>
     </row>
-    <row r="83" spans="1:11" ht="6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:11" ht="6.0" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A83" s="3"/>
       <c r="B83" s="24"/>
       <c r="C83" s="24"/>
@@ -2507,7 +2507,7 @@
       <c r="A84" s="3"/>
       <c r="B84" s="17"/>
       <c r="C84" s="17"/>
-      <c r="D84" s="21" t="s">
+      <c r="D84" t="s" s="21">
         <v>22</v>
       </c>
       <c r="E84" s="22"/>
@@ -2518,7 +2518,7 @@
       <c r="J84" s="66"/>
       <c r="K84" s="4"/>
     </row>
-    <row r="85" spans="1:11" ht="6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:11" ht="6.0" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" s="3"/>
       <c r="B85" s="17"/>
       <c r="C85" s="17"/>
@@ -2535,7 +2535,7 @@
       <c r="A86" s="3"/>
       <c r="B86" s="17"/>
       <c r="C86" s="17"/>
-      <c r="D86" s="21" t="s">
+      <c r="D86" t="s" s="21">
         <v>20</v>
       </c>
       <c r="E86" s="22"/>
@@ -2546,7 +2546,7 @@
       <c r="J86" s="66"/>
       <c r="K86" s="4"/>
     </row>
-    <row r="87" spans="1:11" ht="6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:11" ht="6.0" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A87" s="3"/>
       <c r="B87" s="17"/>
       <c r="C87" s="17"/>
@@ -2563,7 +2563,7 @@
       <c r="A88" s="3"/>
       <c r="B88" s="17"/>
       <c r="C88" s="17"/>
-      <c r="D88" s="21" t="s">
+      <c r="D88" t="s" s="21">
         <v>21</v>
       </c>
       <c r="E88" s="41"/>
@@ -2574,7 +2574,7 @@
       <c r="J88" s="31"/>
       <c r="K88" s="4"/>
     </row>
-    <row r="89" spans="1:11" ht="6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:11" ht="6.0" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A89" s="3"/>
       <c r="B89" s="17"/>
       <c r="C89" s="17"/>
@@ -2591,12 +2591,12 @@
       <c r="A90" s="3"/>
       <c r="B90" s="17"/>
       <c r="C90" s="17"/>
-      <c r="D90" s="23" t="s">
+      <c r="D90" t="s" s="23">
         <v>27</v>
       </c>
       <c r="E90" s="23"/>
       <c r="F90" s="23"/>
-      <c r="G90" s="42" t="b">
+      <c r="G90" t="b" s="42">
         <v>0</v>
       </c>
       <c r="H90" s="43"/>
@@ -2619,7 +2619,7 @@
     </row>
     <row r="92" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A92" s="3"/>
-      <c r="B92" s="21" t="s">
+      <c r="B92" t="s" s="21">
         <v>39</v>
       </c>
       <c r="C92" s="37"/>
@@ -2632,7 +2632,7 @@
       <c r="J92" s="57"/>
       <c r="K92" s="4"/>
     </row>
-    <row r="93" spans="1:11" ht="6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:11" ht="6.0" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A93" s="3"/>
       <c r="B93" s="24"/>
       <c r="C93" s="24"/>
@@ -2645,11 +2645,11 @@
       <c r="J93" s="31"/>
       <c r="K93" s="4"/>
     </row>
-    <row r="94" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:11" ht="15.0" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A94" s="3"/>
       <c r="B94" s="17"/>
       <c r="C94" s="17"/>
-      <c r="D94" s="21" t="s">
+      <c r="D94" t="s" s="21">
         <v>22</v>
       </c>
       <c r="E94" s="22"/>
@@ -2660,7 +2660,7 @@
       <c r="J94" s="66"/>
       <c r="K94" s="4"/>
     </row>
-    <row r="95" spans="1:11" ht="6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:11" ht="6.0" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A95" s="3"/>
       <c r="B95" s="17"/>
       <c r="C95" s="17"/>
@@ -2677,7 +2677,7 @@
       <c r="A96" s="3"/>
       <c r="B96" s="17"/>
       <c r="C96" s="17"/>
-      <c r="D96" s="21" t="s">
+      <c r="D96" t="s" s="21">
         <v>20</v>
       </c>
       <c r="E96" s="22"/>
@@ -2688,7 +2688,7 @@
       <c r="J96" s="66"/>
       <c r="K96" s="4"/>
     </row>
-    <row r="97" spans="1:11" ht="6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:11" ht="6.0" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A97" s="3"/>
       <c r="B97" s="17"/>
       <c r="C97" s="17"/>
@@ -2705,7 +2705,7 @@
       <c r="A98" s="3"/>
       <c r="B98" s="17"/>
       <c r="C98" s="17"/>
-      <c r="D98" s="21" t="s">
+      <c r="D98" t="s" s="21">
         <v>21</v>
       </c>
       <c r="E98" s="41"/>
@@ -2716,7 +2716,7 @@
       <c r="J98" s="31"/>
       <c r="K98" s="4"/>
     </row>
-    <row r="99" spans="1:11" ht="6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:11" ht="6.0" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A99" s="3"/>
       <c r="B99" s="17"/>
       <c r="C99" s="17"/>
@@ -2733,12 +2733,12 @@
       <c r="A100" s="3"/>
       <c r="B100" s="17"/>
       <c r="C100" s="17"/>
-      <c r="D100" s="23" t="s">
+      <c r="D100" t="s" s="23">
         <v>27</v>
       </c>
       <c r="E100" s="23"/>
       <c r="F100" s="23"/>
-      <c r="G100" s="42" t="b">
+      <c r="G100" t="b" s="42">
         <v>0</v>
       </c>
       <c r="H100" s="43"/>
@@ -2746,7 +2746,7 @@
       <c r="J100" s="44"/>
       <c r="K100" s="4"/>
     </row>
-    <row r="101" spans="1:11" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:11" ht="6.0" customHeight="1" x14ac:dyDescent="0.3" thickBot="1">
       <c r="A101" s="5"/>
       <c r="B101" s="19"/>
       <c r="C101" s="19"/>
@@ -2759,7 +2759,7 @@
       <c r="J101" s="27"/>
       <c r="K101" s="6"/>
     </row>
-    <row r="102" spans="1:11" ht="6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:11" ht="6.0" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A102" s="3"/>
       <c r="B102" s="17"/>
       <c r="C102" s="17"/>
@@ -2772,9 +2772,9 @@
       <c r="J102" s="24"/>
       <c r="K102" s="4"/>
     </row>
-    <row r="103" spans="1:11" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:11" ht="18.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A103" s="3"/>
-      <c r="B103" s="20" t="s">
+      <c r="B103" t="s" s="20">
         <v>58</v>
       </c>
       <c r="C103" s="17"/>
@@ -2802,24 +2802,24 @@
     </row>
     <row r="105" spans="1:11" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A105" s="3"/>
-      <c r="B105" s="53" t="s">
+      <c r="B105" t="s" s="53">
         <v>63</v>
       </c>
       <c r="C105" s="25"/>
-      <c r="D105" s="21" t="s">
+      <c r="D105" t="s" s="21">
         <v>53</v>
       </c>
       <c r="E105" s="25"/>
       <c r="F105" s="21"/>
       <c r="G105" s="52"/>
-      <c r="H105" s="21" t="s">
+      <c r="H105" t="s" s="21">
         <v>54</v>
       </c>
       <c r="I105" s="22"/>
       <c r="J105" s="21"/>
       <c r="K105" s="4"/>
     </row>
-    <row r="106" spans="1:11" ht="6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:11" ht="6.0" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A106" s="3"/>
       <c r="B106" s="17"/>
       <c r="C106" s="17"/>
@@ -2836,20 +2836,20 @@
       <c r="A107" s="3"/>
       <c r="B107" s="17"/>
       <c r="C107" s="17"/>
-      <c r="D107" s="21" t="s">
+      <c r="D107" t="s" s="21">
         <v>55</v>
       </c>
       <c r="E107" s="25"/>
       <c r="F107" s="21"/>
       <c r="G107" s="36"/>
-      <c r="H107" s="21" t="s">
+      <c r="H107" t="s" s="21">
         <v>56</v>
       </c>
       <c r="I107" s="22"/>
       <c r="J107" s="21"/>
       <c r="K107" s="4"/>
     </row>
-    <row r="108" spans="1:11" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:11" ht="6.0" customHeight="1" x14ac:dyDescent="0.3" thickBot="1">
       <c r="A108" s="5"/>
       <c r="B108" s="19"/>
       <c r="C108" s="19"/>
@@ -2862,7 +2862,7 @@
       <c r="J108" s="27"/>
       <c r="K108" s="6"/>
     </row>
-    <row r="109" spans="1:11" ht="6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:11" ht="6.0" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A109" s="3"/>
       <c r="B109" s="17"/>
       <c r="C109" s="17"/>
@@ -2875,9 +2875,9 @@
       <c r="J109" s="24"/>
       <c r="K109" s="4"/>
     </row>
-    <row r="110" spans="1:11" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A110" s="3"/>
-      <c r="B110" s="20" t="s">
+      <c r="B110" t="s" s="20">
         <v>59</v>
       </c>
       <c r="C110" s="17"/>
@@ -2905,15 +2905,15 @@
     </row>
     <row r="112" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A112" s="3"/>
-      <c r="B112" s="45" t="s">
+      <c r="B112" t="s" s="45">
         <v>32</v>
       </c>
       <c r="C112" s="17"/>
-      <c r="D112" s="45" t="s">
+      <c r="D112" t="s" s="45">
         <v>15</v>
       </c>
       <c r="E112" s="17"/>
-      <c r="F112" s="21" t="s">
+      <c r="F112" t="s" s="21">
         <v>14</v>
       </c>
       <c r="G112" s="17"/>
@@ -2965,7 +2965,7 @@
       <c r="J115" s="17"/>
       <c r="K115" s="4"/>
     </row>
-    <row r="116" spans="1:11" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:11" ht="6.0" customHeight="1" x14ac:dyDescent="0.3" thickBot="1">
       <c r="A116" s="5"/>
       <c r="B116" s="19"/>
       <c r="C116" s="19"/>
@@ -3057,73 +3057,61 @@
     <col min="3" max="3" width="14.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="33.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="7" t="s">
+    <row r="1" spans="1:3" ht="33.75" customHeight="1" x14ac:dyDescent="0.3" thickBot="1">
+      <c r="A1" t="s" s="7">
         <v>23</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" t="s" s="8">
         <v>24</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" t="s" s="8">
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" ht="22.5" customHeight="1" x14ac:dyDescent="0.3" thickBot="1">
       <c r="A2" s="9">
         <v>0.1</v>
       </c>
-      <c r="B2" s="10" t="s">
+      <c r="B2" t="s" s="10">
         <v>64</v>
       </c>
       <c r="C2" s="11">
         <v>45083</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3" thickBot="1">
       <c r="A3" s="9">
         <v>0.2</v>
       </c>
-      <c r="B3" s="10" t="s">
+      <c r="B3" t="s" s="10">
         <v>65</v>
       </c>
       <c r="C3" s="11">
         <v>45085</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" ht="22.5" customHeight="1" x14ac:dyDescent="0.3" thickBot="1">
       <c r="A4" s="12">
         <v>1</v>
       </c>
-      <c r="B4" s="10" t="s">
+      <c r="B4" t="s" s="10">
         <v>66</v>
       </c>
       <c r="C4" s="11">
         <v>45133</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="36.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" ht="36.75" customHeight="1" x14ac:dyDescent="0.3" thickBot="1">
       <c r="A5" s="9">
         <v>1.1000000000000001</v>
       </c>
-      <c r="B5" s="10" t="s">
+      <c r="B5" t="s" s="10">
         <v>40</v>
       </c>
       <c r="C5" s="11">
         <v>45181</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="7" spans="1:3" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="8" spans="1:3" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="9" spans="1:3" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="10" spans="1:3" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="11" spans="1:3" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="12" spans="1:3" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="13" spans="1:3" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="14" spans="1:3" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="15" spans="1:3" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="16" spans="1:3" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="17" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Now with added tests for #159
</commit_message>
<xml_diff>
--- a/data/customXml.xlsx
+++ b/data/customXml.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/EE85442DAC9CA7A7/Documents/Julia/XLSX/XLSX.jl/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ee85442dac9ca7a7/Documents/Julia/XLSX/XLSX.jl/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="61" documentId="8_{F809508C-CCD6-44EF-B266-70CCB6EF428B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9A8C4B29-9F60-420B-86C7-DB353EBD6FFA}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" tabRatio="604" xr2:uid="{C6551712-42E3-4E24-BA02-CAB261C5432D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" tabRatio="604" activeTab="1" xr2:uid="{C6551712-42E3-4E24-BA02-CAB261C5432D}"/>
   </bookViews>
   <sheets>
     <sheet name="Mock-up" sheetId="1" r:id="rId1"/>
@@ -121,7 +121,7 @@
     <t>Comment</t>
   </si>
   <si>
-    <t xml:space="preserve">Date</t>
+    <t>Date</t>
   </si>
   <si>
     <t>Distributor</t>
@@ -238,7 +238,7 @@
     <t>Competition Details</t>
   </si>
   <si>
-    <t xml:space="preserve">First draft to stimulate feedback</t>
+    <t>First draft to stimulate feedback</t>
   </si>
   <si>
     <t>Revised to show suggested mandatory / optional fields. Changed title.</t>
@@ -312,12 +312,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="8"/>
-      <color rgb="FF000000"/>
-      <name val="Segoe UI"/>
-      <family val="2"/>
-    </font>
-    <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Palatino Linotype"/>
@@ -329,6 +323,12 @@
       <color rgb="FF000000"/>
       <name val="Palatino Linotype"/>
       <family val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="7">
@@ -690,22 +690,22 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="20" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="21" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="23" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="8" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="7" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -840,19 +840,52 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -863,39 +896,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -972,22 +972,13 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="none" lIns="27432" tIns="18288" rIns="0" bIns="0" anchor="t" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="none" lIns="18288" tIns="0" rIns="0" bIns="0" anchor="t" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
                 <a:defRPr sz="1000"/>
               </a:pPr>
-              <a:r>
-                <a:rPr lang="en-GB" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
-                  <a:solidFill>
-                    <a:srgbClr val="000000"/>
-                  </a:solidFill>
-                  <a:latin typeface="Segoe UI"/>
-                  <a:cs typeface="Segoe UI"/>
-                </a:rPr>
-                <a:t/>
-              </a:r>
+              <a:endParaRPr lang="en-GB"/>
             </a:p>
           </xdr:txBody>
         </xdr:sp>
@@ -1301,7 +1292,7 @@
   </sheetPr>
   <dimension ref="A1:K116"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+    <sheetView topLeftCell="A8" workbookViewId="0">
       <selection activeCell="O27" sqref="O27"/>
     </sheetView>
   </sheetViews>
@@ -1436,11 +1427,11 @@
         <v>1</v>
       </c>
       <c r="C9" s="22"/>
-      <c r="D9" s="57"/>
-      <c r="E9" s="57"/>
-      <c r="F9" s="57"/>
-      <c r="G9" s="57"/>
-      <c r="H9" s="57"/>
+      <c r="D9" s="71"/>
+      <c r="E9" s="71"/>
+      <c r="F9" s="71"/>
+      <c r="G9" s="71"/>
+      <c r="H9" s="71"/>
       <c r="I9" s="24"/>
       <c r="J9" s="17"/>
       <c r="K9" s="4"/>
@@ -1464,10 +1455,10 @@
         <v>11</v>
       </c>
       <c r="C11" s="22"/>
-      <c r="D11" s="58"/>
-      <c r="E11" s="59"/>
-      <c r="F11" s="59"/>
-      <c r="G11" s="60"/>
+      <c r="D11" s="57"/>
+      <c r="E11" s="58"/>
+      <c r="F11" s="58"/>
+      <c r="G11" s="59"/>
       <c r="H11" s="17"/>
       <c r="I11" s="17"/>
       <c r="J11" s="13"/>
@@ -1479,10 +1470,10 @@
         <v>12</v>
       </c>
       <c r="C12" s="22"/>
-      <c r="D12" s="58"/>
-      <c r="E12" s="59"/>
-      <c r="F12" s="59"/>
-      <c r="G12" s="60"/>
+      <c r="D12" s="57"/>
+      <c r="E12" s="58"/>
+      <c r="F12" s="58"/>
+      <c r="G12" s="59"/>
       <c r="H12" s="17"/>
       <c r="I12" s="17"/>
       <c r="J12" s="13"/>
@@ -1494,10 +1485,10 @@
         <v>57</v>
       </c>
       <c r="C13" s="22"/>
-      <c r="D13" s="57"/>
-      <c r="E13" s="57"/>
-      <c r="F13" s="57"/>
-      <c r="G13" s="57"/>
+      <c r="D13" s="71"/>
+      <c r="E13" s="71"/>
+      <c r="F13" s="71"/>
+      <c r="G13" s="71"/>
       <c r="H13" s="17"/>
       <c r="I13" s="17"/>
       <c r="J13" s="13"/>
@@ -1509,8 +1500,8 @@
         <v>10</v>
       </c>
       <c r="C14" s="22"/>
-      <c r="D14" s="58"/>
-      <c r="E14" s="60"/>
+      <c r="D14" s="57"/>
+      <c r="E14" s="59"/>
       <c r="F14" s="17"/>
       <c r="G14" s="17"/>
       <c r="H14" s="17"/>
@@ -1537,8 +1528,8 @@
         <v>2</v>
       </c>
       <c r="C16" s="25"/>
-      <c r="D16" s="61"/>
-      <c r="E16" s="62"/>
+      <c r="D16" s="72"/>
+      <c r="E16" s="73"/>
       <c r="F16" s="17"/>
       <c r="G16" s="17"/>
       <c r="H16" s="17"/>
@@ -1565,10 +1556,10 @@
         <v>49</v>
       </c>
       <c r="C18" s="25"/>
-      <c r="D18" t="s" s="63">
+      <c r="D18" t="s" s="74">
         <v>68</v>
       </c>
-      <c r="E18" s="64"/>
+      <c r="E18" s="75"/>
       <c r="F18" s="17"/>
       <c r="G18" s="17"/>
       <c r="H18" t="s" s="21">
@@ -1597,8 +1588,8 @@
         <v>51</v>
       </c>
       <c r="C20" s="25"/>
-      <c r="D20" s="63"/>
-      <c r="E20" s="64"/>
+      <c r="D20" s="74"/>
+      <c r="E20" s="75"/>
       <c r="F20" s="17"/>
       <c r="G20" s="17"/>
       <c r="H20" t="s" s="21">
@@ -1769,9 +1760,9 @@
         <v>26</v>
       </c>
       <c r="C32" s="22"/>
-      <c r="D32" s="57"/>
-      <c r="E32" s="57"/>
-      <c r="F32" s="57"/>
+      <c r="D32" s="71"/>
+      <c r="E32" s="71"/>
+      <c r="F32" s="71"/>
       <c r="G32" s="17"/>
       <c r="H32" s="17"/>
       <c r="I32" s="17"/>
@@ -1797,13 +1788,13 @@
         <v>29</v>
       </c>
       <c r="C34" s="28"/>
-      <c r="D34" s="57"/>
-      <c r="E34" s="57"/>
-      <c r="F34" s="57"/>
-      <c r="G34" s="57"/>
-      <c r="H34" s="57"/>
-      <c r="I34" s="57"/>
-      <c r="J34" s="57"/>
+      <c r="D34" s="71"/>
+      <c r="E34" s="71"/>
+      <c r="F34" s="71"/>
+      <c r="G34" s="71"/>
+      <c r="H34" s="71"/>
+      <c r="I34" s="71"/>
+      <c r="J34" s="71"/>
       <c r="K34" s="4"/>
     </row>
     <row r="35" spans="1:11" ht="6.0" customHeight="1" x14ac:dyDescent="0.25">
@@ -1855,13 +1846,13 @@
         <v>34</v>
       </c>
       <c r="C38" s="28"/>
-      <c r="D38" s="57"/>
-      <c r="E38" s="57"/>
-      <c r="F38" s="57"/>
-      <c r="G38" s="57"/>
-      <c r="H38" s="57"/>
-      <c r="I38" s="57"/>
-      <c r="J38" s="57"/>
+      <c r="D38" s="71"/>
+      <c r="E38" s="71"/>
+      <c r="F38" s="71"/>
+      <c r="G38" s="71"/>
+      <c r="H38" s="71"/>
+      <c r="I38" s="71"/>
+      <c r="J38" s="71"/>
       <c r="K38" s="4"/>
     </row>
     <row r="39" spans="1:11" ht="6.0" customHeight="1" x14ac:dyDescent="0.25">
@@ -1984,11 +1975,11 @@
         <v>37</v>
       </c>
       <c r="C47" s="25"/>
-      <c r="D47" s="57"/>
-      <c r="E47" s="57"/>
-      <c r="F47" s="57"/>
-      <c r="G47" s="57"/>
-      <c r="H47" s="57"/>
+      <c r="D47" s="71"/>
+      <c r="E47" s="71"/>
+      <c r="F47" s="71"/>
+      <c r="G47" s="71"/>
+      <c r="H47" s="71"/>
       <c r="I47" s="17"/>
       <c r="J47" s="32"/>
       <c r="K47" s="4"/>
@@ -2012,11 +2003,11 @@
         <v>36</v>
       </c>
       <c r="C49" s="22"/>
-      <c r="D49" s="58"/>
-      <c r="E49" s="59"/>
-      <c r="F49" s="59"/>
-      <c r="G49" s="59"/>
-      <c r="H49" s="60"/>
+      <c r="D49" s="57"/>
+      <c r="E49" s="58"/>
+      <c r="F49" s="58"/>
+      <c r="G49" s="58"/>
+      <c r="H49" s="59"/>
       <c r="I49" s="24"/>
       <c r="J49" s="32"/>
       <c r="K49" s="4"/>
@@ -2040,41 +2031,41 @@
         <v>7</v>
       </c>
       <c r="C51" s="22"/>
-      <c r="D51" t="s" s="67">
+      <c r="D51" t="s" s="62">
         <v>67</v>
       </c>
-      <c r="E51" s="68"/>
-      <c r="F51" s="68"/>
-      <c r="G51" s="68"/>
-      <c r="H51" s="68"/>
-      <c r="I51" s="68"/>
-      <c r="J51" s="69"/>
+      <c r="E51" s="63"/>
+      <c r="F51" s="63"/>
+      <c r="G51" s="63"/>
+      <c r="H51" s="63"/>
+      <c r="I51" s="63"/>
+      <c r="J51" s="64"/>
       <c r="K51" s="4"/>
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A52" s="3"/>
       <c r="B52" s="17"/>
       <c r="C52" s="17"/>
-      <c r="D52" s="73"/>
-      <c r="E52" s="74"/>
-      <c r="F52" s="74"/>
-      <c r="G52" s="74"/>
-      <c r="H52" s="74"/>
-      <c r="I52" s="74"/>
-      <c r="J52" s="75"/>
+      <c r="D52" s="68"/>
+      <c r="E52" s="69"/>
+      <c r="F52" s="69"/>
+      <c r="G52" s="69"/>
+      <c r="H52" s="69"/>
+      <c r="I52" s="69"/>
+      <c r="J52" s="70"/>
       <c r="K52" s="4"/>
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A53" s="3"/>
       <c r="B53" s="17"/>
       <c r="C53" s="17"/>
-      <c r="D53" s="70"/>
-      <c r="E53" s="71"/>
-      <c r="F53" s="71"/>
-      <c r="G53" s="71"/>
-      <c r="H53" s="71"/>
-      <c r="I53" s="71"/>
-      <c r="J53" s="72"/>
+      <c r="D53" s="65"/>
+      <c r="E53" s="66"/>
+      <c r="F53" s="66"/>
+      <c r="G53" s="66"/>
+      <c r="H53" s="66"/>
+      <c r="I53" s="66"/>
+      <c r="J53" s="67"/>
       <c r="K53" s="4"/>
     </row>
     <row r="54" spans="1:11" x14ac:dyDescent="0.25">
@@ -2096,78 +2087,78 @@
         <v>8</v>
       </c>
       <c r="C55" s="22"/>
-      <c r="D55" s="67"/>
-      <c r="E55" s="68"/>
-      <c r="F55" s="68"/>
-      <c r="G55" s="68"/>
-      <c r="H55" s="68"/>
-      <c r="I55" s="68"/>
-      <c r="J55" s="69"/>
+      <c r="D55" s="62"/>
+      <c r="E55" s="63"/>
+      <c r="F55" s="63"/>
+      <c r="G55" s="63"/>
+      <c r="H55" s="63"/>
+      <c r="I55" s="63"/>
+      <c r="J55" s="64"/>
       <c r="K55" s="4"/>
     </row>
     <row r="56" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A56" s="3"/>
       <c r="B56" s="33"/>
       <c r="C56" s="17"/>
-      <c r="D56" s="73"/>
-      <c r="E56" s="74"/>
-      <c r="F56" s="74"/>
-      <c r="G56" s="74"/>
-      <c r="H56" s="74"/>
-      <c r="I56" s="74"/>
-      <c r="J56" s="75"/>
+      <c r="D56" s="68"/>
+      <c r="E56" s="69"/>
+      <c r="F56" s="69"/>
+      <c r="G56" s="69"/>
+      <c r="H56" s="69"/>
+      <c r="I56" s="69"/>
+      <c r="J56" s="70"/>
       <c r="K56" s="4"/>
     </row>
     <row r="57" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A57" s="3"/>
       <c r="B57" s="33"/>
       <c r="C57" s="17"/>
-      <c r="D57" s="73"/>
-      <c r="E57" s="74"/>
-      <c r="F57" s="74"/>
-      <c r="G57" s="74"/>
-      <c r="H57" s="74"/>
-      <c r="I57" s="74"/>
-      <c r="J57" s="75"/>
+      <c r="D57" s="68"/>
+      <c r="E57" s="69"/>
+      <c r="F57" s="69"/>
+      <c r="G57" s="69"/>
+      <c r="H57" s="69"/>
+      <c r="I57" s="69"/>
+      <c r="J57" s="70"/>
       <c r="K57" s="4"/>
     </row>
     <row r="58" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A58" s="3"/>
       <c r="B58" s="33"/>
       <c r="C58" s="17"/>
-      <c r="D58" s="73"/>
-      <c r="E58" s="74"/>
-      <c r="F58" s="74"/>
-      <c r="G58" s="74"/>
-      <c r="H58" s="74"/>
-      <c r="I58" s="74"/>
-      <c r="J58" s="75"/>
+      <c r="D58" s="68"/>
+      <c r="E58" s="69"/>
+      <c r="F58" s="69"/>
+      <c r="G58" s="69"/>
+      <c r="H58" s="69"/>
+      <c r="I58" s="69"/>
+      <c r="J58" s="70"/>
       <c r="K58" s="4"/>
     </row>
     <row r="59" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A59" s="3"/>
       <c r="B59" s="17"/>
       <c r="C59" s="17"/>
-      <c r="D59" s="73"/>
-      <c r="E59" s="74"/>
-      <c r="F59" s="74"/>
-      <c r="G59" s="74"/>
-      <c r="H59" s="74"/>
-      <c r="I59" s="74"/>
-      <c r="J59" s="75"/>
+      <c r="D59" s="68"/>
+      <c r="E59" s="69"/>
+      <c r="F59" s="69"/>
+      <c r="G59" s="69"/>
+      <c r="H59" s="69"/>
+      <c r="I59" s="69"/>
+      <c r="J59" s="70"/>
       <c r="K59" s="4"/>
     </row>
     <row r="60" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A60" s="3"/>
       <c r="B60" s="17"/>
       <c r="C60" s="17"/>
-      <c r="D60" s="70"/>
-      <c r="E60" s="71"/>
-      <c r="F60" s="71"/>
-      <c r="G60" s="71"/>
-      <c r="H60" s="71"/>
-      <c r="I60" s="71"/>
-      <c r="J60" s="72"/>
+      <c r="D60" s="65"/>
+      <c r="E60" s="66"/>
+      <c r="F60" s="66"/>
+      <c r="G60" s="66"/>
+      <c r="H60" s="66"/>
+      <c r="I60" s="66"/>
+      <c r="J60" s="67"/>
       <c r="K60" s="4"/>
     </row>
     <row r="61" spans="1:11" x14ac:dyDescent="0.25">
@@ -2189,26 +2180,26 @@
         <v>16</v>
       </c>
       <c r="C62" s="22"/>
-      <c r="D62" s="67"/>
-      <c r="E62" s="68"/>
-      <c r="F62" s="68"/>
-      <c r="G62" s="68"/>
-      <c r="H62" s="68"/>
-      <c r="I62" s="68"/>
-      <c r="J62" s="69"/>
+      <c r="D62" s="62"/>
+      <c r="E62" s="63"/>
+      <c r="F62" s="63"/>
+      <c r="G62" s="63"/>
+      <c r="H62" s="63"/>
+      <c r="I62" s="63"/>
+      <c r="J62" s="64"/>
       <c r="K62" s="4"/>
     </row>
     <row r="63" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A63" s="3"/>
       <c r="B63" s="34"/>
       <c r="C63" s="34"/>
-      <c r="D63" s="70"/>
-      <c r="E63" s="71"/>
-      <c r="F63" s="71"/>
-      <c r="G63" s="71"/>
-      <c r="H63" s="71"/>
-      <c r="I63" s="71"/>
-      <c r="J63" s="72"/>
+      <c r="D63" s="65"/>
+      <c r="E63" s="66"/>
+      <c r="F63" s="66"/>
+      <c r="G63" s="66"/>
+      <c r="H63" s="66"/>
+      <c r="I63" s="66"/>
+      <c r="J63" s="67"/>
       <c r="K63" s="4"/>
     </row>
     <row r="64" spans="1:11" ht="6.0" customHeight="1" x14ac:dyDescent="0.25">
@@ -2260,26 +2251,26 @@
         <v>19</v>
       </c>
       <c r="C67" s="22"/>
-      <c r="D67" s="67"/>
-      <c r="E67" s="68"/>
-      <c r="F67" s="68"/>
-      <c r="G67" s="68"/>
-      <c r="H67" s="68"/>
-      <c r="I67" s="68"/>
-      <c r="J67" s="69"/>
+      <c r="D67" s="62"/>
+      <c r="E67" s="63"/>
+      <c r="F67" s="63"/>
+      <c r="G67" s="63"/>
+      <c r="H67" s="63"/>
+      <c r="I67" s="63"/>
+      <c r="J67" s="64"/>
       <c r="K67" s="4"/>
     </row>
     <row r="68" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A68" s="3"/>
       <c r="B68" s="34"/>
       <c r="C68" s="34"/>
-      <c r="D68" s="70"/>
-      <c r="E68" s="71"/>
-      <c r="F68" s="71"/>
-      <c r="G68" s="71"/>
-      <c r="H68" s="71"/>
-      <c r="I68" s="71"/>
-      <c r="J68" s="72"/>
+      <c r="D68" s="65"/>
+      <c r="E68" s="66"/>
+      <c r="F68" s="66"/>
+      <c r="G68" s="66"/>
+      <c r="H68" s="66"/>
+      <c r="I68" s="66"/>
+      <c r="J68" s="67"/>
       <c r="K68" s="4"/>
     </row>
     <row r="69" spans="1:11" ht="6.0" customHeight="1" x14ac:dyDescent="0.25">
@@ -2331,15 +2322,15 @@
         <v>9</v>
       </c>
       <c r="C72" s="22"/>
-      <c r="D72" s="65">
+      <c r="D72" s="60">
         <v>45740</v>
       </c>
-      <c r="E72" s="59"/>
-      <c r="F72" s="59"/>
-      <c r="G72" s="59"/>
-      <c r="H72" s="59"/>
-      <c r="I72" s="59"/>
-      <c r="J72" s="60"/>
+      <c r="E72" s="58"/>
+      <c r="F72" s="58"/>
+      <c r="G72" s="58"/>
+      <c r="H72" s="58"/>
+      <c r="I72" s="58"/>
+      <c r="J72" s="59"/>
       <c r="K72" s="4"/>
     </row>
     <row r="73" spans="1:11" x14ac:dyDescent="0.25">
@@ -2361,13 +2352,13 @@
         <v>13</v>
       </c>
       <c r="C74" s="22"/>
-      <c r="D74" s="57"/>
-      <c r="E74" s="57"/>
-      <c r="F74" s="57"/>
-      <c r="G74" s="57"/>
-      <c r="H74" s="57"/>
-      <c r="I74" s="57"/>
-      <c r="J74" s="57"/>
+      <c r="D74" s="71"/>
+      <c r="E74" s="71"/>
+      <c r="F74" s="71"/>
+      <c r="G74" s="71"/>
+      <c r="H74" s="71"/>
+      <c r="I74" s="71"/>
+      <c r="J74" s="71"/>
       <c r="K74" s="4"/>
     </row>
     <row r="75" spans="1:11" x14ac:dyDescent="0.25">
@@ -2481,13 +2472,13 @@
         <v>38</v>
       </c>
       <c r="C82" s="37"/>
-      <c r="D82" s="57"/>
-      <c r="E82" s="57"/>
-      <c r="F82" s="57"/>
-      <c r="G82" s="57"/>
-      <c r="H82" s="57"/>
-      <c r="I82" s="57"/>
-      <c r="J82" s="57"/>
+      <c r="D82" s="71"/>
+      <c r="E82" s="71"/>
+      <c r="F82" s="71"/>
+      <c r="G82" s="71"/>
+      <c r="H82" s="71"/>
+      <c r="I82" s="71"/>
+      <c r="J82" s="71"/>
       <c r="K82" s="4"/>
     </row>
     <row r="83" spans="1:11" ht="6.0" customHeight="1" x14ac:dyDescent="0.25">
@@ -2511,11 +2502,11 @@
         <v>22</v>
       </c>
       <c r="E84" s="22"/>
-      <c r="F84" s="66"/>
-      <c r="G84" s="66"/>
-      <c r="H84" s="66"/>
-      <c r="I84" s="66"/>
-      <c r="J84" s="66"/>
+      <c r="F84" s="61"/>
+      <c r="G84" s="61"/>
+      <c r="H84" s="61"/>
+      <c r="I84" s="61"/>
+      <c r="J84" s="61"/>
       <c r="K84" s="4"/>
     </row>
     <row r="85" spans="1:11" ht="6.0" customHeight="1" x14ac:dyDescent="0.25">
@@ -2539,11 +2530,11 @@
         <v>20</v>
       </c>
       <c r="E86" s="22"/>
-      <c r="F86" s="66"/>
-      <c r="G86" s="66"/>
-      <c r="H86" s="66"/>
-      <c r="I86" s="66"/>
-      <c r="J86" s="66"/>
+      <c r="F86" s="61"/>
+      <c r="G86" s="61"/>
+      <c r="H86" s="61"/>
+      <c r="I86" s="61"/>
+      <c r="J86" s="61"/>
       <c r="K86" s="4"/>
     </row>
     <row r="87" spans="1:11" ht="6.0" customHeight="1" x14ac:dyDescent="0.25">
@@ -2623,13 +2614,13 @@
         <v>39</v>
       </c>
       <c r="C92" s="37"/>
-      <c r="D92" s="57"/>
-      <c r="E92" s="57"/>
-      <c r="F92" s="57"/>
-      <c r="G92" s="57"/>
-      <c r="H92" s="57"/>
-      <c r="I92" s="57"/>
-      <c r="J92" s="57"/>
+      <c r="D92" s="71"/>
+      <c r="E92" s="71"/>
+      <c r="F92" s="71"/>
+      <c r="G92" s="71"/>
+      <c r="H92" s="71"/>
+      <c r="I92" s="71"/>
+      <c r="J92" s="71"/>
       <c r="K92" s="4"/>
     </row>
     <row r="93" spans="1:11" ht="6.0" customHeight="1" x14ac:dyDescent="0.25">
@@ -2653,11 +2644,11 @@
         <v>22</v>
       </c>
       <c r="E94" s="22"/>
-      <c r="F94" s="66"/>
-      <c r="G94" s="66"/>
-      <c r="H94" s="66"/>
-      <c r="I94" s="66"/>
-      <c r="J94" s="66"/>
+      <c r="F94" s="61"/>
+      <c r="G94" s="61"/>
+      <c r="H94" s="61"/>
+      <c r="I94" s="61"/>
+      <c r="J94" s="61"/>
       <c r="K94" s="4"/>
     </row>
     <row r="95" spans="1:11" ht="6.0" customHeight="1" x14ac:dyDescent="0.25">
@@ -2681,11 +2672,11 @@
         <v>20</v>
       </c>
       <c r="E96" s="22"/>
-      <c r="F96" s="66"/>
-      <c r="G96" s="66"/>
-      <c r="H96" s="66"/>
-      <c r="I96" s="66"/>
-      <c r="J96" s="66"/>
+      <c r="F96" s="61"/>
+      <c r="G96" s="61"/>
+      <c r="H96" s="61"/>
+      <c r="I96" s="61"/>
+      <c r="J96" s="61"/>
       <c r="K96" s="4"/>
     </row>
     <row r="97" spans="1:11" ht="6.0" customHeight="1" x14ac:dyDescent="0.25">
@@ -2980,6 +2971,18 @@
     </row>
   </sheetData>
   <mergeCells count="25">
+    <mergeCell ref="D47:H47"/>
+    <mergeCell ref="D9:H9"/>
+    <mergeCell ref="D11:G11"/>
+    <mergeCell ref="D12:G12"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="D32:F32"/>
+    <mergeCell ref="D38:J38"/>
+    <mergeCell ref="D34:J34"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="D13:G13"/>
     <mergeCell ref="D49:H49"/>
     <mergeCell ref="D72:J72"/>
     <mergeCell ref="F94:J94"/>
@@ -2993,18 +2996,6 @@
     <mergeCell ref="D82:J82"/>
     <mergeCell ref="D74:J74"/>
     <mergeCell ref="D67:J68"/>
-    <mergeCell ref="D47:H47"/>
-    <mergeCell ref="D9:H9"/>
-    <mergeCell ref="D11:G11"/>
-    <mergeCell ref="D12:G12"/>
-    <mergeCell ref="D14:E14"/>
-    <mergeCell ref="D16:E16"/>
-    <mergeCell ref="D32:F32"/>
-    <mergeCell ref="D38:J38"/>
-    <mergeCell ref="D34:J34"/>
-    <mergeCell ref="D18:E18"/>
-    <mergeCell ref="D20:E20"/>
-    <mergeCell ref="D13:G13"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.59055118110236227" right="0.59055118110236227" top="0.19685039370078741" bottom="0.19685039370078741" header="0.31496062992125984" footer="0.31496062992125984"/>
@@ -3044,10 +3035,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{630E29D8-7195-4C2F-809A-EE99FBA98A1B}">
-  <dimension ref="A1:C17"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3118,6 +3109,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101007D73017C158CA1409B57EAC9B77398BC" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="9a938d6d1b800eaa4b55f6ea99a7dd60">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="8fe8bdaf-491a-4d2e-89dd-756120b60898" xmlns:ns3="ed0bb2e3-83d5-46a8-9e95-92c1ca9cc599" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="ad8315b70f40a8e476a692f66bae2bc8" ns2:_="" ns3:_="">
     <xsd:import namespace="8fe8bdaf-491a-4d2e-89dd-756120b60898"/>
@@ -3324,16 +3324,15 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{87A08559-39AD-45D7-9D97-A693167EDA72}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{07773C52-8BED-47F0-AD91-CBF0731BE007}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3350,12 +3349,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{87A08559-39AD-45D7-9D97-A693167EDA72}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Change noDim test to be less brittle
</commit_message>
<xml_diff>
--- a/data/customXml.xlsx
+++ b/data/customXml.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ee85442dac9ca7a7/Documents/Julia/XLSX/XLSX.jl/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/EE85442DAC9CA7A7/Documents/Julia/XLSX/XLSX.jl/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="61" documentId="8_{F809508C-CCD6-44EF-B266-70CCB6EF428B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9A8C4B29-9F60-420B-86C7-DB353EBD6FFA}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" tabRatio="604" activeTab="1" xr2:uid="{C6551712-42E3-4E24-BA02-CAB261C5432D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" tabRatio="604" xr2:uid="{C6551712-42E3-4E24-BA02-CAB261C5432D}"/>
   </bookViews>
   <sheets>
     <sheet name="Mock-up" sheetId="1" r:id="rId1"/>
@@ -121,7 +121,7 @@
     <t>Comment</t>
   </si>
   <si>
-    <t>Date</t>
+    <t xml:space="preserve">Date </t>
   </si>
   <si>
     <t>Distributor</t>
@@ -238,7 +238,7 @@
     <t>Competition Details</t>
   </si>
   <si>
-    <t>First draft to stimulate feedback</t>
+    <t xml:space="preserve">First draft to stimulate feedback </t>
   </si>
   <si>
     <t>Revised to show suggested mandatory / optional fields. Changed title.</t>
@@ -312,6 +312,12 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="8"/>
+      <color rgb="FF000000"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Palatino Linotype"/>
@@ -323,12 +329,6 @@
       <color rgb="FF000000"/>
       <name val="Palatino Linotype"/>
       <family val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="7">
@@ -690,22 +690,22 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="20" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="21" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="23" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="7" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="8" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -840,6 +840,9 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -849,6 +852,18 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="14" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -881,21 +896,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -972,13 +972,22 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="none" lIns="18288" tIns="0" rIns="0" bIns="0" anchor="t" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="none" lIns="27432" tIns="18288" rIns="0" bIns="0" anchor="t" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
                 <a:defRPr sz="1000"/>
               </a:pPr>
-              <a:endParaRPr lang="en-GB"/>
+              <a:r>
+                <a:rPr lang="en-GB" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                  <a:solidFill>
+                    <a:srgbClr val="000000"/>
+                  </a:solidFill>
+                  <a:latin typeface="Segoe UI"/>
+                  <a:cs typeface="Segoe UI"/>
+                </a:rPr>
+                <a:t/>
+              </a:r>
             </a:p>
           </xdr:txBody>
         </xdr:sp>
@@ -1292,7 +1301,7 @@
   </sheetPr>
   <dimension ref="A1:K116"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
       <selection activeCell="O27" sqref="O27"/>
     </sheetView>
   </sheetViews>
@@ -1311,6 +1320,7 @@
     <col min="11" max="11" width="2.7109375" customWidth="1"/>
   </cols>
   <sheetData>
+    <dummy/>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="15"/>
@@ -1427,11 +1437,11 @@
         <v>1</v>
       </c>
       <c r="C9" s="22"/>
-      <c r="D9" s="71"/>
-      <c r="E9" s="71"/>
-      <c r="F9" s="71"/>
-      <c r="G9" s="71"/>
-      <c r="H9" s="71"/>
+      <c r="D9" s="57"/>
+      <c r="E9" s="57"/>
+      <c r="F9" s="57"/>
+      <c r="G9" s="57"/>
+      <c r="H9" s="57"/>
       <c r="I9" s="24"/>
       <c r="J9" s="17"/>
       <c r="K9" s="4"/>
@@ -1455,10 +1465,10 @@
         <v>11</v>
       </c>
       <c r="C11" s="22"/>
-      <c r="D11" s="57"/>
-      <c r="E11" s="58"/>
-      <c r="F11" s="58"/>
-      <c r="G11" s="59"/>
+      <c r="D11" s="58"/>
+      <c r="E11" s="59"/>
+      <c r="F11" s="59"/>
+      <c r="G11" s="60"/>
       <c r="H11" s="17"/>
       <c r="I11" s="17"/>
       <c r="J11" s="13"/>
@@ -1470,10 +1480,10 @@
         <v>12</v>
       </c>
       <c r="C12" s="22"/>
-      <c r="D12" s="57"/>
-      <c r="E12" s="58"/>
-      <c r="F12" s="58"/>
-      <c r="G12" s="59"/>
+      <c r="D12" s="58"/>
+      <c r="E12" s="59"/>
+      <c r="F12" s="59"/>
+      <c r="G12" s="60"/>
       <c r="H12" s="17"/>
       <c r="I12" s="17"/>
       <c r="J12" s="13"/>
@@ -1485,10 +1495,10 @@
         <v>57</v>
       </c>
       <c r="C13" s="22"/>
-      <c r="D13" s="71"/>
-      <c r="E13" s="71"/>
-      <c r="F13" s="71"/>
-      <c r="G13" s="71"/>
+      <c r="D13" s="57"/>
+      <c r="E13" s="57"/>
+      <c r="F13" s="57"/>
+      <c r="G13" s="57"/>
       <c r="H13" s="17"/>
       <c r="I13" s="17"/>
       <c r="J13" s="13"/>
@@ -1500,8 +1510,8 @@
         <v>10</v>
       </c>
       <c r="C14" s="22"/>
-      <c r="D14" s="57"/>
-      <c r="E14" s="59"/>
+      <c r="D14" s="58"/>
+      <c r="E14" s="60"/>
       <c r="F14" s="17"/>
       <c r="G14" s="17"/>
       <c r="H14" s="17"/>
@@ -1528,8 +1538,8 @@
         <v>2</v>
       </c>
       <c r="C16" s="25"/>
-      <c r="D16" s="72"/>
-      <c r="E16" s="73"/>
+      <c r="D16" s="61"/>
+      <c r="E16" s="62"/>
       <c r="F16" s="17"/>
       <c r="G16" s="17"/>
       <c r="H16" s="17"/>
@@ -1556,10 +1566,10 @@
         <v>49</v>
       </c>
       <c r="C18" s="25"/>
-      <c r="D18" t="s" s="74">
+      <c r="D18" t="s" s="63">
         <v>68</v>
       </c>
-      <c r="E18" s="75"/>
+      <c r="E18" s="64"/>
       <c r="F18" s="17"/>
       <c r="G18" s="17"/>
       <c r="H18" t="s" s="21">
@@ -1588,8 +1598,8 @@
         <v>51</v>
       </c>
       <c r="C20" s="25"/>
-      <c r="D20" s="74"/>
-      <c r="E20" s="75"/>
+      <c r="D20" s="63"/>
+      <c r="E20" s="64"/>
       <c r="F20" s="17"/>
       <c r="G20" s="17"/>
       <c r="H20" t="s" s="21">
@@ -1760,9 +1770,9 @@
         <v>26</v>
       </c>
       <c r="C32" s="22"/>
-      <c r="D32" s="71"/>
-      <c r="E32" s="71"/>
-      <c r="F32" s="71"/>
+      <c r="D32" s="57"/>
+      <c r="E32" s="57"/>
+      <c r="F32" s="57"/>
       <c r="G32" s="17"/>
       <c r="H32" s="17"/>
       <c r="I32" s="17"/>
@@ -1788,13 +1798,13 @@
         <v>29</v>
       </c>
       <c r="C34" s="28"/>
-      <c r="D34" s="71"/>
-      <c r="E34" s="71"/>
-      <c r="F34" s="71"/>
-      <c r="G34" s="71"/>
-      <c r="H34" s="71"/>
-      <c r="I34" s="71"/>
-      <c r="J34" s="71"/>
+      <c r="D34" s="57"/>
+      <c r="E34" s="57"/>
+      <c r="F34" s="57"/>
+      <c r="G34" s="57"/>
+      <c r="H34" s="57"/>
+      <c r="I34" s="57"/>
+      <c r="J34" s="57"/>
       <c r="K34" s="4"/>
     </row>
     <row r="35" spans="1:11" ht="6.0" customHeight="1" x14ac:dyDescent="0.25">
@@ -1846,13 +1856,13 @@
         <v>34</v>
       </c>
       <c r="C38" s="28"/>
-      <c r="D38" s="71"/>
-      <c r="E38" s="71"/>
-      <c r="F38" s="71"/>
-      <c r="G38" s="71"/>
-      <c r="H38" s="71"/>
-      <c r="I38" s="71"/>
-      <c r="J38" s="71"/>
+      <c r="D38" s="57"/>
+      <c r="E38" s="57"/>
+      <c r="F38" s="57"/>
+      <c r="G38" s="57"/>
+      <c r="H38" s="57"/>
+      <c r="I38" s="57"/>
+      <c r="J38" s="57"/>
       <c r="K38" s="4"/>
     </row>
     <row r="39" spans="1:11" ht="6.0" customHeight="1" x14ac:dyDescent="0.25">
@@ -1975,11 +1985,11 @@
         <v>37</v>
       </c>
       <c r="C47" s="25"/>
-      <c r="D47" s="71"/>
-      <c r="E47" s="71"/>
-      <c r="F47" s="71"/>
-      <c r="G47" s="71"/>
-      <c r="H47" s="71"/>
+      <c r="D47" s="57"/>
+      <c r="E47" s="57"/>
+      <c r="F47" s="57"/>
+      <c r="G47" s="57"/>
+      <c r="H47" s="57"/>
       <c r="I47" s="17"/>
       <c r="J47" s="32"/>
       <c r="K47" s="4"/>
@@ -2003,11 +2013,11 @@
         <v>36</v>
       </c>
       <c r="C49" s="22"/>
-      <c r="D49" s="57"/>
-      <c r="E49" s="58"/>
-      <c r="F49" s="58"/>
-      <c r="G49" s="58"/>
-      <c r="H49" s="59"/>
+      <c r="D49" s="58"/>
+      <c r="E49" s="59"/>
+      <c r="F49" s="59"/>
+      <c r="G49" s="59"/>
+      <c r="H49" s="60"/>
       <c r="I49" s="24"/>
       <c r="J49" s="32"/>
       <c r="K49" s="4"/>
@@ -2031,41 +2041,41 @@
         <v>7</v>
       </c>
       <c r="C51" s="22"/>
-      <c r="D51" t="s" s="62">
+      <c r="D51" t="s" s="67">
         <v>67</v>
       </c>
-      <c r="E51" s="63"/>
-      <c r="F51" s="63"/>
-      <c r="G51" s="63"/>
-      <c r="H51" s="63"/>
-      <c r="I51" s="63"/>
-      <c r="J51" s="64"/>
+      <c r="E51" s="68"/>
+      <c r="F51" s="68"/>
+      <c r="G51" s="68"/>
+      <c r="H51" s="68"/>
+      <c r="I51" s="68"/>
+      <c r="J51" s="69"/>
       <c r="K51" s="4"/>
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A52" s="3"/>
       <c r="B52" s="17"/>
       <c r="C52" s="17"/>
-      <c r="D52" s="68"/>
-      <c r="E52" s="69"/>
-      <c r="F52" s="69"/>
-      <c r="G52" s="69"/>
-      <c r="H52" s="69"/>
-      <c r="I52" s="69"/>
-      <c r="J52" s="70"/>
+      <c r="D52" s="73"/>
+      <c r="E52" s="74"/>
+      <c r="F52" s="74"/>
+      <c r="G52" s="74"/>
+      <c r="H52" s="74"/>
+      <c r="I52" s="74"/>
+      <c r="J52" s="75"/>
       <c r="K52" s="4"/>
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A53" s="3"/>
       <c r="B53" s="17"/>
       <c r="C53" s="17"/>
-      <c r="D53" s="65"/>
-      <c r="E53" s="66"/>
-      <c r="F53" s="66"/>
-      <c r="G53" s="66"/>
-      <c r="H53" s="66"/>
-      <c r="I53" s="66"/>
-      <c r="J53" s="67"/>
+      <c r="D53" s="70"/>
+      <c r="E53" s="71"/>
+      <c r="F53" s="71"/>
+      <c r="G53" s="71"/>
+      <c r="H53" s="71"/>
+      <c r="I53" s="71"/>
+      <c r="J53" s="72"/>
       <c r="K53" s="4"/>
     </row>
     <row r="54" spans="1:11" x14ac:dyDescent="0.25">
@@ -2087,78 +2097,78 @@
         <v>8</v>
       </c>
       <c r="C55" s="22"/>
-      <c r="D55" s="62"/>
-      <c r="E55" s="63"/>
-      <c r="F55" s="63"/>
-      <c r="G55" s="63"/>
-      <c r="H55" s="63"/>
-      <c r="I55" s="63"/>
-      <c r="J55" s="64"/>
+      <c r="D55" s="67"/>
+      <c r="E55" s="68"/>
+      <c r="F55" s="68"/>
+      <c r="G55" s="68"/>
+      <c r="H55" s="68"/>
+      <c r="I55" s="68"/>
+      <c r="J55" s="69"/>
       <c r="K55" s="4"/>
     </row>
     <row r="56" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A56" s="3"/>
       <c r="B56" s="33"/>
       <c r="C56" s="17"/>
-      <c r="D56" s="68"/>
-      <c r="E56" s="69"/>
-      <c r="F56" s="69"/>
-      <c r="G56" s="69"/>
-      <c r="H56" s="69"/>
-      <c r="I56" s="69"/>
-      <c r="J56" s="70"/>
+      <c r="D56" s="73"/>
+      <c r="E56" s="74"/>
+      <c r="F56" s="74"/>
+      <c r="G56" s="74"/>
+      <c r="H56" s="74"/>
+      <c r="I56" s="74"/>
+      <c r="J56" s="75"/>
       <c r="K56" s="4"/>
     </row>
     <row r="57" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A57" s="3"/>
       <c r="B57" s="33"/>
       <c r="C57" s="17"/>
-      <c r="D57" s="68"/>
-      <c r="E57" s="69"/>
-      <c r="F57" s="69"/>
-      <c r="G57" s="69"/>
-      <c r="H57" s="69"/>
-      <c r="I57" s="69"/>
-      <c r="J57" s="70"/>
+      <c r="D57" s="73"/>
+      <c r="E57" s="74"/>
+      <c r="F57" s="74"/>
+      <c r="G57" s="74"/>
+      <c r="H57" s="74"/>
+      <c r="I57" s="74"/>
+      <c r="J57" s="75"/>
       <c r="K57" s="4"/>
     </row>
     <row r="58" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A58" s="3"/>
       <c r="B58" s="33"/>
       <c r="C58" s="17"/>
-      <c r="D58" s="68"/>
-      <c r="E58" s="69"/>
-      <c r="F58" s="69"/>
-      <c r="G58" s="69"/>
-      <c r="H58" s="69"/>
-      <c r="I58" s="69"/>
-      <c r="J58" s="70"/>
+      <c r="D58" s="73"/>
+      <c r="E58" s="74"/>
+      <c r="F58" s="74"/>
+      <c r="G58" s="74"/>
+      <c r="H58" s="74"/>
+      <c r="I58" s="74"/>
+      <c r="J58" s="75"/>
       <c r="K58" s="4"/>
     </row>
     <row r="59" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A59" s="3"/>
       <c r="B59" s="17"/>
       <c r="C59" s="17"/>
-      <c r="D59" s="68"/>
-      <c r="E59" s="69"/>
-      <c r="F59" s="69"/>
-      <c r="G59" s="69"/>
-      <c r="H59" s="69"/>
-      <c r="I59" s="69"/>
-      <c r="J59" s="70"/>
+      <c r="D59" s="73"/>
+      <c r="E59" s="74"/>
+      <c r="F59" s="74"/>
+      <c r="G59" s="74"/>
+      <c r="H59" s="74"/>
+      <c r="I59" s="74"/>
+      <c r="J59" s="75"/>
       <c r="K59" s="4"/>
     </row>
     <row r="60" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A60" s="3"/>
       <c r="B60" s="17"/>
       <c r="C60" s="17"/>
-      <c r="D60" s="65"/>
-      <c r="E60" s="66"/>
-      <c r="F60" s="66"/>
-      <c r="G60" s="66"/>
-      <c r="H60" s="66"/>
-      <c r="I60" s="66"/>
-      <c r="J60" s="67"/>
+      <c r="D60" s="70"/>
+      <c r="E60" s="71"/>
+      <c r="F60" s="71"/>
+      <c r="G60" s="71"/>
+      <c r="H60" s="71"/>
+      <c r="I60" s="71"/>
+      <c r="J60" s="72"/>
       <c r="K60" s="4"/>
     </row>
     <row r="61" spans="1:11" x14ac:dyDescent="0.25">
@@ -2180,26 +2190,26 @@
         <v>16</v>
       </c>
       <c r="C62" s="22"/>
-      <c r="D62" s="62"/>
-      <c r="E62" s="63"/>
-      <c r="F62" s="63"/>
-      <c r="G62" s="63"/>
-      <c r="H62" s="63"/>
-      <c r="I62" s="63"/>
-      <c r="J62" s="64"/>
+      <c r="D62" s="67"/>
+      <c r="E62" s="68"/>
+      <c r="F62" s="68"/>
+      <c r="G62" s="68"/>
+      <c r="H62" s="68"/>
+      <c r="I62" s="68"/>
+      <c r="J62" s="69"/>
       <c r="K62" s="4"/>
     </row>
     <row r="63" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A63" s="3"/>
       <c r="B63" s="34"/>
       <c r="C63" s="34"/>
-      <c r="D63" s="65"/>
-      <c r="E63" s="66"/>
-      <c r="F63" s="66"/>
-      <c r="G63" s="66"/>
-      <c r="H63" s="66"/>
-      <c r="I63" s="66"/>
-      <c r="J63" s="67"/>
+      <c r="D63" s="70"/>
+      <c r="E63" s="71"/>
+      <c r="F63" s="71"/>
+      <c r="G63" s="71"/>
+      <c r="H63" s="71"/>
+      <c r="I63" s="71"/>
+      <c r="J63" s="72"/>
       <c r="K63" s="4"/>
     </row>
     <row r="64" spans="1:11" ht="6.0" customHeight="1" x14ac:dyDescent="0.25">
@@ -2251,26 +2261,26 @@
         <v>19</v>
       </c>
       <c r="C67" s="22"/>
-      <c r="D67" s="62"/>
-      <c r="E67" s="63"/>
-      <c r="F67" s="63"/>
-      <c r="G67" s="63"/>
-      <c r="H67" s="63"/>
-      <c r="I67" s="63"/>
-      <c r="J67" s="64"/>
+      <c r="D67" s="67"/>
+      <c r="E67" s="68"/>
+      <c r="F67" s="68"/>
+      <c r="G67" s="68"/>
+      <c r="H67" s="68"/>
+      <c r="I67" s="68"/>
+      <c r="J67" s="69"/>
       <c r="K67" s="4"/>
     </row>
     <row r="68" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A68" s="3"/>
       <c r="B68" s="34"/>
       <c r="C68" s="34"/>
-      <c r="D68" s="65"/>
-      <c r="E68" s="66"/>
-      <c r="F68" s="66"/>
-      <c r="G68" s="66"/>
-      <c r="H68" s="66"/>
-      <c r="I68" s="66"/>
-      <c r="J68" s="67"/>
+      <c r="D68" s="70"/>
+      <c r="E68" s="71"/>
+      <c r="F68" s="71"/>
+      <c r="G68" s="71"/>
+      <c r="H68" s="71"/>
+      <c r="I68" s="71"/>
+      <c r="J68" s="72"/>
       <c r="K68" s="4"/>
     </row>
     <row r="69" spans="1:11" ht="6.0" customHeight="1" x14ac:dyDescent="0.25">
@@ -2322,15 +2332,15 @@
         <v>9</v>
       </c>
       <c r="C72" s="22"/>
-      <c r="D72" s="60">
+      <c r="D72" s="65">
         <v>45740</v>
       </c>
-      <c r="E72" s="58"/>
-      <c r="F72" s="58"/>
-      <c r="G72" s="58"/>
-      <c r="H72" s="58"/>
-      <c r="I72" s="58"/>
-      <c r="J72" s="59"/>
+      <c r="E72" s="59"/>
+      <c r="F72" s="59"/>
+      <c r="G72" s="59"/>
+      <c r="H72" s="59"/>
+      <c r="I72" s="59"/>
+      <c r="J72" s="60"/>
       <c r="K72" s="4"/>
     </row>
     <row r="73" spans="1:11" x14ac:dyDescent="0.25">
@@ -2352,13 +2362,13 @@
         <v>13</v>
       </c>
       <c r="C74" s="22"/>
-      <c r="D74" s="71"/>
-      <c r="E74" s="71"/>
-      <c r="F74" s="71"/>
-      <c r="G74" s="71"/>
-      <c r="H74" s="71"/>
-      <c r="I74" s="71"/>
-      <c r="J74" s="71"/>
+      <c r="D74" s="57"/>
+      <c r="E74" s="57"/>
+      <c r="F74" s="57"/>
+      <c r="G74" s="57"/>
+      <c r="H74" s="57"/>
+      <c r="I74" s="57"/>
+      <c r="J74" s="57"/>
       <c r="K74" s="4"/>
     </row>
     <row r="75" spans="1:11" x14ac:dyDescent="0.25">
@@ -2472,13 +2482,13 @@
         <v>38</v>
       </c>
       <c r="C82" s="37"/>
-      <c r="D82" s="71"/>
-      <c r="E82" s="71"/>
-      <c r="F82" s="71"/>
-      <c r="G82" s="71"/>
-      <c r="H82" s="71"/>
-      <c r="I82" s="71"/>
-      <c r="J82" s="71"/>
+      <c r="D82" s="57"/>
+      <c r="E82" s="57"/>
+      <c r="F82" s="57"/>
+      <c r="G82" s="57"/>
+      <c r="H82" s="57"/>
+      <c r="I82" s="57"/>
+      <c r="J82" s="57"/>
       <c r="K82" s="4"/>
     </row>
     <row r="83" spans="1:11" ht="6.0" customHeight="1" x14ac:dyDescent="0.25">
@@ -2502,11 +2512,11 @@
         <v>22</v>
       </c>
       <c r="E84" s="22"/>
-      <c r="F84" s="61"/>
-      <c r="G84" s="61"/>
-      <c r="H84" s="61"/>
-      <c r="I84" s="61"/>
-      <c r="J84" s="61"/>
+      <c r="F84" s="66"/>
+      <c r="G84" s="66"/>
+      <c r="H84" s="66"/>
+      <c r="I84" s="66"/>
+      <c r="J84" s="66"/>
       <c r="K84" s="4"/>
     </row>
     <row r="85" spans="1:11" ht="6.0" customHeight="1" x14ac:dyDescent="0.25">
@@ -2530,11 +2540,11 @@
         <v>20</v>
       </c>
       <c r="E86" s="22"/>
-      <c r="F86" s="61"/>
-      <c r="G86" s="61"/>
-      <c r="H86" s="61"/>
-      <c r="I86" s="61"/>
-      <c r="J86" s="61"/>
+      <c r="F86" s="66"/>
+      <c r="G86" s="66"/>
+      <c r="H86" s="66"/>
+      <c r="I86" s="66"/>
+      <c r="J86" s="66"/>
       <c r="K86" s="4"/>
     </row>
     <row r="87" spans="1:11" ht="6.0" customHeight="1" x14ac:dyDescent="0.25">
@@ -2614,13 +2624,13 @@
         <v>39</v>
       </c>
       <c r="C92" s="37"/>
-      <c r="D92" s="71"/>
-      <c r="E92" s="71"/>
-      <c r="F92" s="71"/>
-      <c r="G92" s="71"/>
-      <c r="H92" s="71"/>
-      <c r="I92" s="71"/>
-      <c r="J92" s="71"/>
+      <c r="D92" s="57"/>
+      <c r="E92" s="57"/>
+      <c r="F92" s="57"/>
+      <c r="G92" s="57"/>
+      <c r="H92" s="57"/>
+      <c r="I92" s="57"/>
+      <c r="J92" s="57"/>
       <c r="K92" s="4"/>
     </row>
     <row r="93" spans="1:11" ht="6.0" customHeight="1" x14ac:dyDescent="0.25">
@@ -2644,11 +2654,11 @@
         <v>22</v>
       </c>
       <c r="E94" s="22"/>
-      <c r="F94" s="61"/>
-      <c r="G94" s="61"/>
-      <c r="H94" s="61"/>
-      <c r="I94" s="61"/>
-      <c r="J94" s="61"/>
+      <c r="F94" s="66"/>
+      <c r="G94" s="66"/>
+      <c r="H94" s="66"/>
+      <c r="I94" s="66"/>
+      <c r="J94" s="66"/>
       <c r="K94" s="4"/>
     </row>
     <row r="95" spans="1:11" ht="6.0" customHeight="1" x14ac:dyDescent="0.25">
@@ -2672,11 +2682,11 @@
         <v>20</v>
       </c>
       <c r="E96" s="22"/>
-      <c r="F96" s="61"/>
-      <c r="G96" s="61"/>
-      <c r="H96" s="61"/>
-      <c r="I96" s="61"/>
-      <c r="J96" s="61"/>
+      <c r="F96" s="66"/>
+      <c r="G96" s="66"/>
+      <c r="H96" s="66"/>
+      <c r="I96" s="66"/>
+      <c r="J96" s="66"/>
       <c r="K96" s="4"/>
     </row>
     <row r="97" spans="1:11" ht="6.0" customHeight="1" x14ac:dyDescent="0.25">
@@ -2971,18 +2981,6 @@
     </row>
   </sheetData>
   <mergeCells count="25">
-    <mergeCell ref="D47:H47"/>
-    <mergeCell ref="D9:H9"/>
-    <mergeCell ref="D11:G11"/>
-    <mergeCell ref="D12:G12"/>
-    <mergeCell ref="D14:E14"/>
-    <mergeCell ref="D16:E16"/>
-    <mergeCell ref="D32:F32"/>
-    <mergeCell ref="D38:J38"/>
-    <mergeCell ref="D34:J34"/>
-    <mergeCell ref="D18:E18"/>
-    <mergeCell ref="D20:E20"/>
-    <mergeCell ref="D13:G13"/>
     <mergeCell ref="D49:H49"/>
     <mergeCell ref="D72:J72"/>
     <mergeCell ref="F94:J94"/>
@@ -2996,6 +2994,18 @@
     <mergeCell ref="D82:J82"/>
     <mergeCell ref="D74:J74"/>
     <mergeCell ref="D67:J68"/>
+    <mergeCell ref="D47:H47"/>
+    <mergeCell ref="D9:H9"/>
+    <mergeCell ref="D11:G11"/>
+    <mergeCell ref="D12:G12"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="D32:F32"/>
+    <mergeCell ref="D38:J38"/>
+    <mergeCell ref="D34:J34"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="D13:G13"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.59055118110236227" right="0.59055118110236227" top="0.19685039370078741" bottom="0.19685039370078741" header="0.31496062992125984" footer="0.31496062992125984"/>
@@ -3035,10 +3045,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{630E29D8-7195-4C2F-809A-EE99FBA98A1B}">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3048,7 +3058,8 @@
     <col min="3" max="3" width="14.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="33.75" customHeight="1" x14ac:dyDescent="0.3" thickBot="1">
+    <dummy/>
+    <row r="1" spans="1:3" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s" s="7">
         <v>23</v>
       </c>
@@ -3059,7 +3070,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="22.5" customHeight="1" x14ac:dyDescent="0.3" thickBot="1">
+    <row r="2" spans="1:3" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="9">
         <v>0.1</v>
       </c>
@@ -3081,7 +3092,7 @@
         <v>45085</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="22.5" customHeight="1" x14ac:dyDescent="0.3" thickBot="1">
+    <row r="4" spans="1:3" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="12">
         <v>1</v>
       </c>
@@ -3092,7 +3103,7 @@
         <v>45133</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="36.75" customHeight="1" x14ac:dyDescent="0.3" thickBot="1">
+    <row r="5" spans="1:3" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="9">
         <v>1.1000000000000001</v>
       </c>
@@ -3109,15 +3120,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101007D73017C158CA1409B57EAC9B77398BC" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="9a938d6d1b800eaa4b55f6ea99a7dd60">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="8fe8bdaf-491a-4d2e-89dd-756120b60898" xmlns:ns3="ed0bb2e3-83d5-46a8-9e95-92c1ca9cc599" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="ad8315b70f40a8e476a692f66bae2bc8" ns2:_="" ns3:_="">
     <xsd:import namespace="8fe8bdaf-491a-4d2e-89dd-756120b60898"/>
@@ -3324,15 +3326,16 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{87A08559-39AD-45D7-9D97-A693167EDA72}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{07773C52-8BED-47F0-AD91-CBF0731BE007}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3349,4 +3352,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{87A08559-39AD-45D7-9D97-A693167EDA72}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>